<commit_message>
Actualización de archivos JSON y scripts 3 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_Colmedica.xlsx
+++ b/Segumiento_Colmedica.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="197">
   <si>
     <t>Asignado a</t>
   </si>
@@ -215,10 +215,17 @@
     <t>Crear servicio para que Colmedica entregue a Imagine el XML y el numero de solicitud, y se almacene al interior para luego hacer la lectura segun req 306</t>
   </si>
   <si>
+    <t>PRUEBAS COLMEDICA</t>
+  </si>
+  <si>
     <t>24/06/2025 Nuevo - Cliente
 07/08/2025 Se define parámetros de entrada más estructura de tabla en base de datos
 08/08/2025 Se comienza a crear WS con REST de tipo POST
-08/08/2025 Se realiza ajustes adicionales para el guardado de XML y el guardado de la información en base de datos</t>
+08/08/2025 Se realiza ajustes adicionales para el guardado de XML y el guardado de la información en base de datos
+14/08/2025 Jennifer envía correo al cliente para que se haga la prueba respectiva de conexión, entregando documentación y url en servidor de pruebas
+19/08/2025 El cliente informa de una inconsistencia, en la que el consumo le devuelve el error {"response":false,"message":"Error al guardar el archivo XML"} 
+21/08/2025 Se realiza la correccion, en Pruebas hizo falta el permiso a una carpeta
+26/08/2025 Jennifer informa al Cliente por correo electrónico del error corregido, y que pueden continuar haciendo pruebas</t>
   </si>
   <si>
     <t>verificacion cuentas contables - Cuentas Medicas UMD (valor cuentas contables)</t>
@@ -406,14 +413,16 @@
     <t>OPT_7</t>
   </si>
   <si>
-    <t>Afiliaciones POS - Estados de Salud (Muestra Militar)</t>
+    <t>Afiliaciones POS - PRE - Estados de Salud (Muestra Militar)</t>
   </si>
   <si>
     <t>Ya con los estados de salud capturados, 1. Crear tarea programada para identificar las solicitudes a diario de la muestra militar del del 15%.de lo validado en el día por el proceso automático.
 2. Se debe crear una opción como bandeja de trabajo donde se liste la muestra militar  , para que una persona realice a revisión control de calidad</t>
   </si>
   <si>
-    <t>28/08/2025 Se inicia con el desarrollo, se cerea opción en menu Imagine para crear la bandeja de trabajo - Muestra Militar Estados de SAlud</t>
+    <t>28/08/2025 Se inicia con el desarrollo, pagina con la que se debe sacar la muestra militar del 20% y dejar en una tabla marcadas para revisar
+1/09/2025 pagina de tarea programada terminada, para sacar la muestra e insertar en tabla destino
+2/09/2025 se genera documentacion tecnica, y se inicia con el desarrollo de la bandeja de trabajo para revisar las solicitudes de la muestra</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2987,7 +2996,7 @@
       <c r="L7" s="49"/>
       <c r="M7" s="38">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32770</v>
+        <v>32772</v>
       </c>
       <c r="N7" s="50"/>
       <c r="O7" s="51"/>
@@ -3049,7 +3058,7 @@
       <c r="L8" s="54"/>
       <c r="M8" s="24">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>32770</v>
+        <v>32772</v>
       </c>
       <c r="N8" s="54"/>
       <c r="O8" s="55"/>
@@ -3097,7 +3106,7 @@
       </c>
       <c r="E9" s="56"/>
       <c r="F9" s="33" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G9" s="34">
         <v>99.0</v>
@@ -3126,7 +3135,7 @@
       </c>
       <c r="O9" s="51"/>
       <c r="P9" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="42" t="b">
         <v>1</v>
@@ -3162,10 +3171,10 @@
         <v>304.0</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="18" t="s">
@@ -3198,7 +3207,7 @@
         <v>45805.0</v>
       </c>
       <c r="P10" s="46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="26" t="b">
         <v>1</v>
@@ -3231,13 +3240,13 @@
         <v>17</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="62" t="s">
@@ -3272,7 +3281,7 @@
         <v>45890.0</v>
       </c>
       <c r="P11" s="41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="42" t="b">
         <v>1</v>
@@ -3305,13 +3314,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E12" s="65"/>
       <c r="F12" s="66" t="s">
@@ -3333,14 +3342,14 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N12" s="54"/>
       <c r="O12" s="60">
         <v>45807.0</v>
       </c>
       <c r="P12" s="46" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q12" s="26" t="b">
         <v>1</v>
@@ -3373,13 +3382,13 @@
         <v>36</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E13" s="68"/>
       <c r="F13" s="69" t="s">
@@ -3412,7 +3421,7 @@
         <v>45835.0</v>
       </c>
       <c r="P13" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q13" s="42" t="b">
         <v>1</v>
@@ -3445,13 +3454,13 @@
         <v>36</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" s="70"/>
       <c r="F14" s="66" t="s">
@@ -3484,7 +3493,7 @@
         <v>45849.0</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="26" t="b">
         <v>1</v>
@@ -3517,13 +3526,13 @@
         <v>36</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E15" s="71"/>
       <c r="F15" s="69" t="s">
@@ -3556,7 +3565,7 @@
         <v>45859.0</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q15" s="42" t="b">
         <v>1</v>
@@ -3589,13 +3598,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="66" t="s">
@@ -3611,12 +3620,12 @@
       <c r="L16" s="54"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32770</v>
+        <v>32772</v>
       </c>
       <c r="N16" s="54"/>
       <c r="O16" s="60"/>
       <c r="P16" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q16" s="26" t="b">
         <v>1</v>
@@ -3649,13 +3658,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="69" t="s">
@@ -3690,7 +3699,7 @@
         <v>45847.0</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q17" s="42" t="b">
         <v>1</v>
@@ -3723,13 +3732,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="73" t="s">
@@ -3764,7 +3773,7 @@
         <v>45896.0</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="26" t="b">
         <v>1</v>
@@ -3800,10 +3809,10 @@
         <v>311.0</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="77"/>
       <c r="F19" s="62" t="s">
@@ -3834,7 +3843,7 @@
         <v>45881.0</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q19" s="42" t="b">
         <v>1</v>
@@ -3870,17 +3879,17 @@
         <v>312.0</v>
       </c>
       <c r="C20" s="79" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D20" s="80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E20" s="81"/>
       <c r="F20" s="73" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="74">
-        <v>2.0</v>
+        <v>100.0</v>
       </c>
       <c r="H20" s="74">
         <v>2.0</v>
@@ -3908,7 +3917,7 @@
         <v>45895.0</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q20" s="26" t="b">
         <v>1</v>
@@ -3941,17 +3950,17 @@
         <v>36</v>
       </c>
       <c r="B21" s="84" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="77"/>
       <c r="F21" s="62" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G21" s="85">
         <v>90.0</v>
@@ -3978,7 +3987,7 @@
       </c>
       <c r="O21" s="51"/>
       <c r="P21" s="41" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q21" s="42" t="b">
         <v>1</v>
@@ -4011,10 +4020,10 @@
         <v>36</v>
       </c>
       <c r="B22" s="89" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="81"/>
@@ -4031,7 +4040,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>32770</v>
+        <v>32772</v>
       </c>
       <c r="N22" s="59"/>
       <c r="O22" s="55"/>
@@ -4067,20 +4076,20 @@
         <v>36</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="77"/>
       <c r="F23" s="62" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G23" s="85">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="H23" s="85">
         <v>3.0</v>
@@ -4091,16 +4100,18 @@
       <c r="J23" s="87">
         <v>45897.0</v>
       </c>
-      <c r="K23" s="49"/>
+      <c r="K23" s="57">
+        <v>45903.0</v>
+      </c>
       <c r="L23" s="49"/>
       <c r="M23" s="38">
         <f>IF(ISBLANK(L23), NETWORKDAYS(J23, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J23, L23, Hoja2!$A$1:$A$18))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N23" s="50"/>
       <c r="O23" s="51"/>
       <c r="P23" s="41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q23" s="42" t="b">
         <v>1</v>
@@ -41733,11 +41744,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="F2:F940">
+      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L940 N2:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F940">
-      <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS COLMEDICA,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -41775,7 +41786,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="156" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" s="156" t="s">
         <v>2</v>
@@ -41802,13 +41813,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="159" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K1" s="156" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L1" s="160" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M1" s="161"/>
       <c r="N1" s="161"/>
@@ -41827,14 +41838,14 @@
     </row>
     <row r="2">
       <c r="A2" s="162" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B2" s="163" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C2" s="164"/>
       <c r="D2" s="165" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E2" s="166">
         <v>45526.0</v>
@@ -41848,7 +41859,7 @@
       <c r="J2" s="164"/>
       <c r="K2" s="164"/>
       <c r="L2" s="164" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M2" s="167"/>
       <c r="N2" s="167"/>
@@ -41867,13 +41878,13 @@
     </row>
     <row r="3">
       <c r="A3" s="168" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B3" s="169" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="170" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D3" s="170" t="s">
         <v>20</v>
@@ -41897,7 +41908,7 @@
       </c>
       <c r="K3" s="172"/>
       <c r="L3" s="174" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M3" s="161"/>
       <c r="N3" s="161"/>
@@ -41916,16 +41927,16 @@
     </row>
     <row r="4">
       <c r="A4" s="175" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B4" s="176" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C4" s="175" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D4" s="177" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E4" s="178">
         <v>45581.0</v>
@@ -41948,7 +41959,7 @@
       </c>
       <c r="K4" s="178"/>
       <c r="L4" s="175" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M4" s="181"/>
       <c r="N4" s="181"/>
@@ -41967,16 +41978,16 @@
     </row>
     <row r="5">
       <c r="A5" s="160" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="176" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C5" s="170" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" s="182" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E5" s="171">
         <v>45572.0</v>
@@ -41997,7 +42008,7 @@
       </c>
       <c r="K5" s="171"/>
       <c r="L5" s="174" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M5" s="161"/>
       <c r="N5" s="161"/>
@@ -42016,16 +42027,16 @@
     </row>
     <row r="6">
       <c r="A6" s="183" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="183" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="177" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D6" s="183" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E6" s="184">
         <v>45602.0</v>
@@ -42046,7 +42057,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="185" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M6" s="186"/>
       <c r="N6" s="187"/>
@@ -42065,16 +42076,16 @@
     </row>
     <row r="7">
       <c r="A7" s="160" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B7" s="169" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7" s="188" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D7" s="182" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E7" s="171">
         <v>45589.0</v>
@@ -42095,7 +42106,7 @@
       </c>
       <c r="K7" s="182"/>
       <c r="L7" s="190" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M7" s="191"/>
       <c r="N7" s="191"/>
@@ -42114,14 +42125,14 @@
     </row>
     <row r="8">
       <c r="A8" s="192" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B8" s="193" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C8" s="194"/>
       <c r="D8" s="194" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" s="195">
         <v>45603.0</v>
@@ -42142,7 +42153,7 @@
       </c>
       <c r="K8" s="195"/>
       <c r="L8" s="197" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M8" s="161"/>
       <c r="N8" s="161"/>
@@ -42161,16 +42172,16 @@
     </row>
     <row r="9">
       <c r="A9" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" s="199" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" s="200" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D9" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E9" s="202">
         <v>45671.0</v>
@@ -42179,7 +42190,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="200" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H9" s="202">
         <v>45680.0</v>
@@ -42193,7 +42204,7 @@
       </c>
       <c r="K9" s="200"/>
       <c r="L9" s="204" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M9" s="205"/>
       <c r="N9" s="205"/>
@@ -42212,14 +42223,14 @@
     </row>
     <row r="10">
       <c r="A10" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B10" s="206"/>
       <c r="C10" s="204" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D10" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E10" s="202">
         <v>45671.0</v>
@@ -42238,7 +42249,7 @@
       <c r="J10" s="200"/>
       <c r="K10" s="200"/>
       <c r="L10" s="204" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M10" s="205"/>
       <c r="N10" s="205"/>
@@ -42257,14 +42268,14 @@
     </row>
     <row r="11">
       <c r="A11" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B11" s="206"/>
       <c r="C11" s="204" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E11" s="202">
         <v>45671.0</v>
@@ -42283,7 +42294,7 @@
       <c r="J11" s="200"/>
       <c r="K11" s="200"/>
       <c r="L11" s="204" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M11" s="205"/>
       <c r="N11" s="205"/>
@@ -42302,14 +42313,14 @@
     </row>
     <row r="12">
       <c r="A12" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B12" s="206"/>
       <c r="C12" s="204" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D12" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E12" s="202">
         <v>45671.0</v>
@@ -42328,7 +42339,7 @@
       <c r="J12" s="200"/>
       <c r="K12" s="200"/>
       <c r="L12" s="204" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M12" s="205"/>
       <c r="N12" s="205"/>
@@ -42347,14 +42358,14 @@
     </row>
     <row r="13">
       <c r="A13" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" s="206"/>
       <c r="C13" s="204" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D13" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E13" s="202">
         <v>45671.0</v>
@@ -42373,7 +42384,7 @@
       <c r="J13" s="200"/>
       <c r="K13" s="200"/>
       <c r="L13" s="204" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M13" s="205"/>
       <c r="N13" s="205"/>
@@ -42392,14 +42403,14 @@
     </row>
     <row r="14">
       <c r="A14" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="206"/>
       <c r="C14" s="204" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D14" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E14" s="202">
         <v>45671.0</v>
@@ -42418,7 +42429,7 @@
       <c r="J14" s="200"/>
       <c r="K14" s="200"/>
       <c r="L14" s="200" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M14" s="205"/>
       <c r="N14" s="205"/>
@@ -42437,14 +42448,14 @@
     </row>
     <row r="15">
       <c r="A15" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B15" s="206"/>
       <c r="C15" s="204" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D15" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E15" s="202">
         <v>45671.0</v>
@@ -42463,7 +42474,7 @@
       <c r="J15" s="200"/>
       <c r="K15" s="200"/>
       <c r="L15" s="200" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M15" s="205"/>
       <c r="N15" s="205"/>
@@ -42482,14 +42493,14 @@
     </row>
     <row r="16">
       <c r="A16" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B16" s="207"/>
       <c r="C16" s="208" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D16" s="201" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E16" s="202">
         <v>45681.0</v>
@@ -42508,7 +42519,7 @@
       <c r="J16" s="200"/>
       <c r="K16" s="200"/>
       <c r="L16" s="204" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M16" s="205"/>
       <c r="N16" s="205"/>
@@ -49044,7 +49055,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="205" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49052,7 +49063,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="205" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49060,7 +49071,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="205" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49068,7 +49079,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="205" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49076,7 +49087,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="205" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49084,7 +49095,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="205" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49092,7 +49103,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="205" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49100,7 +49111,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="205" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49108,7 +49119,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="205" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49116,7 +49127,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="205" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49124,7 +49135,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="205" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49132,7 +49143,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="205" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49140,7 +49151,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="205" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49148,7 +49159,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="205" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49156,7 +49167,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="205" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49164,7 +49175,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="205" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49172,7 +49183,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="205" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49180,7 +49191,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="205" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50196,7 +50207,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="210" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="205"/>
       <c r="C1" s="205"/>
@@ -50254,7 +50265,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="211" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="212">
         <v>45596.0</v>
@@ -50547,261 +50558,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="215" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B4" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C4" s="217" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="218" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="218" t="s">
-        <v>163</v>
-      </c>
       <c r="E4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O4" s="218" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P4" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U4" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE4" s="220" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK4" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL4" s="220" t="s">
+        <v>169</v>
+      </c>
+      <c r="AM4" s="218" t="s">
         <v>167</v>
       </c>
-      <c r="AF4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AG4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AH4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AI4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK4" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL4" s="220" t="s">
-        <v>168</v>
-      </c>
-      <c r="AM4" s="218" t="s">
-        <v>166</v>
-      </c>
       <c r="AN4" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AO4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP4" s="220" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AQ4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS4" s="220" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AT4" s="221" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AV4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY4" s="220" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AZ4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI4" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ4" s="220" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="BK4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BL4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BM4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BN4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BO4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BP4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BQ4" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BR4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CD4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG4" s="218"/>
       <c r="CH4" s="218"/>
       <c r="CI4" s="220" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="CJ4" s="218"/>
       <c r="CK4" s="218"/>
@@ -50813,249 +50824,249 @@
       <c r="CQ4" s="218"/>
       <c r="CR4" s="218"/>
       <c r="CS4" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="215" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P5" s="219" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U5" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="V5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE5" s="222"/>
       <c r="AF5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL5" s="222"/>
       <c r="AM5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP5" s="222"/>
       <c r="AQ5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AR5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AS5" s="222"/>
       <c r="AT5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AU5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AV5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AW5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AX5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AY5" s="222"/>
       <c r="AZ5" s="218" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BA5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI5" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ5" s="222"/>
       <c r="BK5" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL5" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN5" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BP5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CD5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG5" s="218"/>
       <c r="CH5" s="218"/>
@@ -51070,249 +51081,249 @@
       <c r="CQ5" s="218"/>
       <c r="CR5" s="218"/>
       <c r="CS5" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="215" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K6" s="223" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O6" s="218" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="V6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE6" s="222"/>
       <c r="AF6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL6" s="222"/>
       <c r="AM6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP6" s="222"/>
       <c r="AQ6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS6" s="222"/>
       <c r="AT6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AV6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY6" s="222"/>
       <c r="AZ6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ6" s="222"/>
       <c r="BK6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM6" s="218" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="BN6" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BP6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CD6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG6" s="218"/>
       <c r="CH6" s="218"/>
@@ -51327,198 +51338,198 @@
       <c r="CQ6" s="218"/>
       <c r="CR6" s="218"/>
       <c r="CS6" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="215" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L7" s="223" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O7" s="218" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P7" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U7" s="219" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="V7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z7" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AA7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE7" s="222"/>
       <c r="AF7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL7" s="222"/>
       <c r="AM7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP7" s="222"/>
       <c r="AQ7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS7" s="222"/>
       <c r="AT7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU7" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AV7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY7" s="222"/>
       <c r="AZ7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI7" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ7" s="222"/>
       <c r="BK7" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL7" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN7" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO7" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BP7" s="218"/>
       <c r="BQ7" s="218"/>
@@ -51526,16 +51537,16 @@
       <c r="BS7" s="218"/>
       <c r="BT7" s="218"/>
       <c r="BU7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX7" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY7" s="218"/>
       <c r="BZ7" s="218"/>
@@ -51561,220 +51572,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="215" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L8" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="M8" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="O8" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="M8" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="N8" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="O8" s="218" t="s">
-        <v>165</v>
-      </c>
       <c r="P8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="V8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W8" s="218" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="X8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB8" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE8" s="222"/>
       <c r="AF8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL8" s="222"/>
       <c r="AM8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN8" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AO8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP8" s="222"/>
       <c r="AQ8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS8" s="222"/>
       <c r="AT8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AV8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY8" s="222"/>
       <c r="AZ8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG8" s="218" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="BH8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ8" s="222"/>
       <c r="BK8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN8" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BP8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW8" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX8" s="218" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BY8" s="218"/>
       <c r="BZ8" s="218"/>
@@ -51800,244 +51811,244 @@
     </row>
     <row r="9">
       <c r="A9" s="215" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B9" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O9" s="223" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="V9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE9" s="222"/>
       <c r="AF9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL9" s="222"/>
       <c r="AM9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP9" s="222"/>
       <c r="AQ9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS9" s="222"/>
       <c r="AT9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AV9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY9" s="222"/>
       <c r="AZ9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ9" s="222"/>
       <c r="BK9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN9" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BP9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CD9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG9" s="218"/>
       <c r="CH9" s="218"/>
@@ -52052,249 +52063,249 @@
       <c r="CQ9" s="218"/>
       <c r="CR9" s="218"/>
       <c r="CS9" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="215" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B10" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I10" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="L10" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="M10" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="N10" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="O10" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="J10" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="K10" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="L10" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="M10" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="N10" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="O10" s="218" t="s">
-        <v>165</v>
-      </c>
       <c r="P10" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="R10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U10" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AE10" s="222"/>
       <c r="AF10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AL10" s="222"/>
       <c r="AM10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AN10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP10" s="222"/>
       <c r="AQ10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS10" s="222"/>
       <c r="AT10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AV10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY10" s="222"/>
       <c r="AZ10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BA10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BB10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BC10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BD10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BE10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BF10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BG10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BH10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI10" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ10" s="222"/>
       <c r="BK10" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL10" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN10" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BP10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW10" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BX10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CD10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG10" s="218"/>
       <c r="CH10" s="218"/>
@@ -52309,249 +52320,249 @@
       <c r="CQ10" s="218"/>
       <c r="CR10" s="218"/>
       <c r="CS10" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="215" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B11" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J11" s="218" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K11" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="L11" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="M11" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="N11" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="O11" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="M11" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="N11" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="O11" s="218" t="s">
-        <v>165</v>
-      </c>
       <c r="P11" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="S11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="T11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U11" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Z11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AC11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AE11" s="222"/>
       <c r="AF11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AH11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AI11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL11" s="222"/>
       <c r="AM11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AN11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AO11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP11" s="222"/>
       <c r="AQ11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AR11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AS11" s="222"/>
       <c r="AT11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AU11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AV11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AW11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AY11" s="222"/>
       <c r="AZ11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BA11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BB11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BF11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BG11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BH11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI11" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BJ11" s="222"/>
       <c r="BK11" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BL11" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN11" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BO11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BP11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BQ11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BR11" s="218" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="BS11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BT11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BU11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BX11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BY11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CA11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CB11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CC11" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CD11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG11" s="218"/>
       <c r="CH11" s="218"/>
@@ -52566,249 +52577,249 @@
       <c r="CQ11" s="218"/>
       <c r="CR11" s="218"/>
       <c r="CS11" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="215" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B12" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="J12" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="K12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="L12" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="M12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="O12" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="G12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="I12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="J12" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="K12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="L12" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="M12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="N12" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="O12" s="218" t="s">
-        <v>165</v>
-      </c>
       <c r="P12" s="219" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Q12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="R12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="S12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="T12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U12" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="W12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Y12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Z12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AA12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AB12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AE12" s="222"/>
       <c r="AF12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AG12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AH12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AI12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AJ12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AK12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL12" s="222"/>
       <c r="AM12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AN12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AO12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AP12" s="222"/>
       <c r="AQ12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AR12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AS12" s="222"/>
       <c r="AT12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AU12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AV12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AW12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AX12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AY12" s="222"/>
       <c r="AZ12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BA12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BB12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BC12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BD12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BE12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BF12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BG12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BH12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BI12" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BJ12" s="222"/>
       <c r="BK12" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BL12" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BM12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BN12" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BO12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BP12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BQ12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BR12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BS12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BT12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BU12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BV12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BW12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BX12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BY12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BZ12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CA12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CB12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CC12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CD12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CE12" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CG12" s="218"/>
       <c r="CH12" s="218"/>
@@ -52823,249 +52834,249 @@
       <c r="CQ12" s="218"/>
       <c r="CR12" s="218"/>
       <c r="CS12" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="215" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B13" s="216" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="I13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="L13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="M13" s="218" t="s">
+        <v>164</v>
+      </c>
+      <c r="N13" s="218" t="s">
+        <v>167</v>
+      </c>
+      <c r="O13" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="H13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="I13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="J13" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="K13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="L13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="M13" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="N13" s="218" t="s">
-        <v>166</v>
-      </c>
-      <c r="O13" s="218" t="s">
-        <v>165</v>
-      </c>
       <c r="P13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="R13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="S13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="T13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="V13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="W13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Y13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Z13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AA13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AB13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AE13" s="224"/>
       <c r="AF13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AG13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AH13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AI13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AJ13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AK13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AL13" s="224"/>
       <c r="AM13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AN13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AO13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AP13" s="224"/>
       <c r="AQ13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AR13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AS13" s="224"/>
       <c r="AT13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AU13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AV13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AW13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AX13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AY13" s="224"/>
       <c r="AZ13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BA13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BB13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BC13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BD13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BE13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BF13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BG13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BH13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BI13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BJ13" s="224"/>
       <c r="BK13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BL13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BM13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BN13" s="219" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BO13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BP13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BQ13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BR13" s="218" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="BS13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BT13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BU13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BV13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BW13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BX13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BY13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BZ13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CA13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CB13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CC13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="CD13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CE13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CF13" s="218" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="CG13" s="218"/>
       <c r="CH13" s="218"/>
@@ -53080,7 +53091,7 @@
       <c r="CQ13" s="218"/>
       <c r="CR13" s="218"/>
       <c r="CS13" s="218" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54106,7 +54117,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="225" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" s="225" t="s">
         <v>2</v>
@@ -54133,13 +54144,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="229" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K1" s="230" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L1" s="228" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M1" s="231"/>
       <c r="N1" s="231"/>
@@ -54158,10 +54169,10 @@
     </row>
     <row r="2">
       <c r="A2" s="232" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="233" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C2" s="234"/>
       <c r="D2" s="234" t="s">
@@ -54188,7 +54199,7 @@
       </c>
       <c r="K2" s="237"/>
       <c r="L2" s="238" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M2" s="231"/>
       <c r="N2" s="231"/>
@@ -54207,13 +54218,13 @@
     </row>
     <row r="3">
       <c r="A3" s="232" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B3" s="239" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C3" s="240" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D3" s="234" t="s">
         <v>39</v>
@@ -54235,7 +54246,7 @@
       </c>
       <c r="K3" s="235"/>
       <c r="L3" s="238" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M3" s="241"/>
       <c r="N3" s="231"/>
@@ -54254,11 +54265,11 @@
     </row>
     <row r="4">
       <c r="A4" s="232" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B4" s="222"/>
       <c r="C4" s="242" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D4" s="234" t="s">
         <v>39</v>
@@ -54280,7 +54291,7 @@
       </c>
       <c r="K4" s="243"/>
       <c r="L4" s="246" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M4" s="241"/>
       <c r="N4" s="231"/>
@@ -54299,13 +54310,13 @@
     </row>
     <row r="5">
       <c r="A5" s="232" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B5" s="228" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C5" s="234" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D5" s="234" t="s">
         <v>39</v>
@@ -54327,7 +54338,7 @@
       </c>
       <c r="K5" s="235"/>
       <c r="L5" s="238" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M5" s="241"/>
       <c r="N5" s="231"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 17 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_Colmedica.xlsx
+++ b/Segumiento_Colmedica.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="220">
   <si>
     <t>Asignado a</t>
   </si>
@@ -400,10 +400,16 @@
     <t>Afiliaciones PRE - Generacion de Kits</t>
   </si>
   <si>
+    <t>Cambiar la plataforma del Access - Crear archivos planos enviados al proveedor que hace el envío de los Kits a los clientes de medicina prepagada, a partir del correo que ya se envía de confirmación del cargue de las preexistencias. Si todo esta Cargado, generar archivos planos, conectarse a la ruta y dejar los archivos, enviar correo notificando de la generación. En caso de que las preexistencias no esten todas cargadas, no se genera nada autmático, sin embargo se dispondrá una opción desde el Sitio Web de Imagine para que se generen dihos archivos.</t>
+  </si>
+  <si>
     <t>EN PROCESO</t>
   </si>
   <si>
-    <t>9/09/2025 Se inicia con el levantamiento de información</t>
+    <t xml:space="preserve">9/09/2025 Se inicia con el levantamiento de información para iniciar con el desarrollo
+11/09/2025 Creación de schema-tabla principal - el resto se revisarán si son necesarias o como se ajusta seguramente se puedan omitir
+12/09/2025 Se inicia el desarrollo para traer la información (Pagina principal - página de funciones)
+16/09/2025 </t>
   </si>
   <si>
     <t>OPT_7</t>
@@ -422,7 +428,8 @@
 3/09/2025 Se adelantó la bandeja de trabajo, ya se listan las solicitudes de la muestra, mostrando la información para realizar la validación.
 4/09/2025 se termina el desarrollo
 5/09/2025 se pasa a pruebas, tanto paginas nuevas, como las modificadas por funciones, y creacion de tablas
-8/09/2025 se pasa a aproduccion, tanto paginas nuevas, como las modificadas por funciones, y creacion de tablas. se deja la tarea programada para la extracción de la muestra</t>
+8/09/2025 se pasa a aproduccion, tanto paginas nuevas, como las modificadas por funciones, y creacion de tablas. se deja la tarea programada para la extracción de la muestra
+15/09/2025 se corre histórico desde el 1/08/2025 de muestra a la fecha 14/09, desde el 15/09 queda habilitada la tarea programada 8/09. Se genera documentación Técnica</t>
   </si>
   <si>
     <t>OPT_8</t>
@@ -502,7 +509,8 @@
 Adicional una vez almacenada esta información se debe cerrar el registro, invocando pag \var\www\html\modulo_imagine\core\imagine\indexaprocesosafiliaciones.php opcion 6, la cual deja el registro tramitado</t>
   </si>
   <si>
-    <t>15/09/2025 Se realiza lectura ocr para recuperar estacals del archivo PDF</t>
+    <t>15/09/2025 Se realiza lectura ocr para recuperar estacals del archivo PDF
+16/09/2025 Relizar el servicio para la lectura del PDF y guardado en la base de datos</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2734,7 +2742,7 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32780</v>
+        <v>32782</v>
       </c>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
@@ -2796,7 +2804,7 @@
       <c r="L8" s="24"/>
       <c r="M8" s="25">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>32780</v>
+        <v>32782</v>
       </c>
       <c r="N8" s="24"/>
       <c r="O8" s="24"/>
@@ -3080,7 +3088,7 @@
       <c r="L12" s="24"/>
       <c r="M12" s="25">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N12" s="24"/>
       <c r="O12" s="24">
@@ -3358,7 +3366,7 @@
       <c r="L16" s="24"/>
       <c r="M16" s="25">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32780</v>
+        <v>32782</v>
       </c>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
@@ -3763,13 +3771,15 @@
       <c r="C22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="E22" s="18"/>
       <c r="F22" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G22" s="20">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="22">
@@ -3782,12 +3792,12 @@
       <c r="L22" s="24"/>
       <c r="M22" s="25">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Q22" s="12" t="b">
         <v>1</v>
@@ -3820,13 +3830,13 @@
         <v>36</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="19" t="s">
@@ -3861,7 +3871,7 @@
         <v>45908.0</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q23" s="12" t="b">
         <v>1</v>
@@ -3894,17 +3904,17 @@
         <v>17</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G24" s="20">
         <v>60.0</v>
@@ -3922,12 +3932,12 @@
       <c r="L24" s="24"/>
       <c r="M24" s="25">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
       <c r="P24" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q24" s="12" t="b">
         <v>1</v>
@@ -3960,13 +3970,13 @@
         <v>17</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="19" t="s">
@@ -4001,7 +4011,7 @@
         <v>45909.0</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q25" s="12" t="b">
         <v>1</v>
@@ -4032,14 +4042,16 @@
     <row r="26">
       <c r="A26" s="14"/>
       <c r="B26" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="I26" s="22">
@@ -4048,7 +4060,10 @@
       <c r="J26" s="23"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
-      <c r="M26" s="25"/>
+      <c r="M26" s="25">
+        <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
+        <v>32782</v>
+      </c>
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="26"/>
@@ -4083,13 +4098,13 @@
         <v>17</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="19" t="s">
@@ -4111,8 +4126,9 @@
       <c r="L27" s="29">
         <v>45912.0</v>
       </c>
-      <c r="M27" s="29">
-        <v>45912.0</v>
+      <c r="M27" s="25">
+        <f>IF(ISBLANK(L27), NETWORKDAYS(J27, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J27, L27, Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
       </c>
       <c r="N27" s="29">
         <v>45912.0</v>
@@ -4121,7 +4137,7 @@
         <v>45912.0</v>
       </c>
       <c r="P27" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q27" s="12" t="b">
         <v>1</v>
@@ -4155,22 +4171,27 @@
         <v>315.0</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E28" s="18"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
       <c r="I28" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J28" s="23"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
+      <c r="M28" s="25">
+        <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
+        <v>32782</v>
+      </c>
       <c r="N28" s="24"/>
       <c r="O28" s="24"/>
       <c r="P28" s="26"/>
@@ -4206,22 +4227,27 @@
         <v>314.0</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
+      <c r="F29" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="G29" s="20"/>
       <c r="H29" s="21"/>
       <c r="I29" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J29" s="23"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
-      <c r="M29" s="25"/>
+      <c r="M29" s="25">
+        <f>IF(ISBLANK(L29), NETWORKDAYS(J29, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J29, L29, Hoja2!$A$1:$A$18))</f>
+        <v>32782</v>
+      </c>
       <c r="N29" s="24"/>
       <c r="O29" s="24"/>
       <c r="P29" s="26"/>
@@ -4259,30 +4285,43 @@
         <v>313.0</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
+        <v>92</v>
+      </c>
+      <c r="G30" s="20">
+        <v>10.0</v>
+      </c>
+      <c r="H30" s="21">
+        <v>3.0</v>
+      </c>
       <c r="I30" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J30" s="23">
         <v>45912.0</v>
       </c>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="24"/>
+      <c r="K30" s="24">
+        <v>45918.0</v>
+      </c>
+      <c r="L30" s="24">
+        <v>45917.0</v>
+      </c>
+      <c r="M30" s="25">
+        <f>IF(ISBLANK(L30), NETWORKDAYS(J30, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J30, L30, Hoja2!$A$1:$A$18))</f>
+        <v>4</v>
+      </c>
+      <c r="N30" s="24">
+        <v>45917.0</v>
+      </c>
       <c r="O30" s="24"/>
       <c r="P30" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q30" s="12" t="b">
         <v>1</v>
@@ -41672,7 +41711,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="70" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="70" t="s">
         <v>2</v>
@@ -41699,13 +41738,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="73" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K1" s="70" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L1" s="74" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M1" s="75"/>
       <c r="N1" s="75"/>
@@ -41724,14 +41763,14 @@
     </row>
     <row r="2">
       <c r="A2" s="76" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="78"/>
       <c r="D2" s="79" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E2" s="80">
         <v>45526.0</v>
@@ -41745,7 +41784,7 @@
       <c r="J2" s="78"/>
       <c r="K2" s="78"/>
       <c r="L2" s="78" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M2" s="81"/>
       <c r="N2" s="81"/>
@@ -41764,13 +41803,13 @@
     </row>
     <row r="3">
       <c r="A3" s="82" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C3" s="84" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D3" s="84" t="s">
         <v>20</v>
@@ -41794,7 +41833,7 @@
       </c>
       <c r="K3" s="86"/>
       <c r="L3" s="88" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M3" s="75"/>
       <c r="N3" s="75"/>
@@ -41813,16 +41852,16 @@
     </row>
     <row r="4">
       <c r="A4" s="89" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E4" s="92">
         <v>45581.0</v>
@@ -41845,7 +41884,7 @@
       </c>
       <c r="K4" s="92"/>
       <c r="L4" s="89" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M4" s="95"/>
       <c r="N4" s="95"/>
@@ -41864,16 +41903,16 @@
     </row>
     <row r="5">
       <c r="A5" s="74" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E5" s="85">
         <v>45572.0</v>
@@ -41894,7 +41933,7 @@
       </c>
       <c r="K5" s="85"/>
       <c r="L5" s="88" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M5" s="75"/>
       <c r="N5" s="75"/>
@@ -41913,16 +41952,16 @@
     </row>
     <row r="6">
       <c r="A6" s="97" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D6" s="97" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E6" s="98">
         <v>45602.0</v>
@@ -41943,7 +41982,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="99" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M6" s="100"/>
       <c r="N6" s="101"/>
@@ -41962,16 +42001,16 @@
     </row>
     <row r="7">
       <c r="A7" s="74" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="102" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E7" s="85">
         <v>45589.0</v>
@@ -41992,7 +42031,7 @@
       </c>
       <c r="K7" s="96"/>
       <c r="L7" s="104" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M7" s="105"/>
       <c r="N7" s="105"/>
@@ -42011,14 +42050,14 @@
     </row>
     <row r="8">
       <c r="A8" s="106" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" s="107" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C8" s="108"/>
       <c r="D8" s="108" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E8" s="109">
         <v>45603.0</v>
@@ -42039,7 +42078,7 @@
       </c>
       <c r="K8" s="109"/>
       <c r="L8" s="111" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M8" s="75"/>
       <c r="N8" s="75"/>
@@ -42058,16 +42097,16 @@
     </row>
     <row r="9">
       <c r="A9" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B9" s="113" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C9" s="114" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D9" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E9" s="116">
         <v>45671.0</v>
@@ -42076,7 +42115,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H9" s="116">
         <v>45680.0</v>
@@ -42090,7 +42129,7 @@
       </c>
       <c r="K9" s="114"/>
       <c r="L9" s="118" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M9" s="119"/>
       <c r="N9" s="119"/>
@@ -42109,14 +42148,14 @@
     </row>
     <row r="10">
       <c r="A10" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B10" s="120"/>
       <c r="C10" s="118" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D10" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E10" s="116">
         <v>45671.0</v>
@@ -42135,7 +42174,7 @@
       <c r="J10" s="114"/>
       <c r="K10" s="114"/>
       <c r="L10" s="118" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M10" s="119"/>
       <c r="N10" s="119"/>
@@ -42154,14 +42193,14 @@
     </row>
     <row r="11">
       <c r="A11" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="120"/>
       <c r="C11" s="118" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E11" s="116">
         <v>45671.0</v>
@@ -42180,7 +42219,7 @@
       <c r="J11" s="114"/>
       <c r="K11" s="114"/>
       <c r="L11" s="118" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M11" s="119"/>
       <c r="N11" s="119"/>
@@ -42199,14 +42238,14 @@
     </row>
     <row r="12">
       <c r="A12" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" s="120"/>
       <c r="C12" s="118" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E12" s="116">
         <v>45671.0</v>
@@ -42225,7 +42264,7 @@
       <c r="J12" s="114"/>
       <c r="K12" s="114"/>
       <c r="L12" s="118" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M12" s="119"/>
       <c r="N12" s="119"/>
@@ -42244,14 +42283,14 @@
     </row>
     <row r="13">
       <c r="A13" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B13" s="120"/>
       <c r="C13" s="118" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D13" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E13" s="116">
         <v>45671.0</v>
@@ -42270,7 +42309,7 @@
       <c r="J13" s="114"/>
       <c r="K13" s="114"/>
       <c r="L13" s="118" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M13" s="119"/>
       <c r="N13" s="119"/>
@@ -42289,14 +42328,14 @@
     </row>
     <row r="14">
       <c r="A14" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B14" s="120"/>
       <c r="C14" s="118" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E14" s="116">
         <v>45671.0</v>
@@ -42315,7 +42354,7 @@
       <c r="J14" s="114"/>
       <c r="K14" s="114"/>
       <c r="L14" s="114" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M14" s="119"/>
       <c r="N14" s="119"/>
@@ -42334,14 +42373,14 @@
     </row>
     <row r="15">
       <c r="A15" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B15" s="120"/>
       <c r="C15" s="118" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E15" s="116">
         <v>45671.0</v>
@@ -42360,7 +42399,7 @@
       <c r="J15" s="114"/>
       <c r="K15" s="114"/>
       <c r="L15" s="114" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M15" s="119"/>
       <c r="N15" s="119"/>
@@ -42379,14 +42418,14 @@
     </row>
     <row r="16">
       <c r="A16" s="112" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B16" s="121"/>
       <c r="C16" s="122" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D16" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E16" s="116">
         <v>45681.0</v>
@@ -42405,7 +42444,7 @@
       <c r="J16" s="114"/>
       <c r="K16" s="114"/>
       <c r="L16" s="118" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M16" s="119"/>
       <c r="N16" s="119"/>
@@ -48941,7 +48980,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -48949,7 +48988,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="119" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -48957,7 +48996,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -48965,7 +49004,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="119" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -48973,7 +49012,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="119" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -48981,7 +49020,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -48989,7 +49028,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="119" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -48997,7 +49036,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49005,7 +49044,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49013,7 +49052,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49021,7 +49060,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="119" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49029,7 +49068,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="119" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49037,7 +49076,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="119" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49045,7 +49084,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="119" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49053,7 +49092,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="119" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49061,7 +49100,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="119" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49069,7 +49108,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="119" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49077,7 +49116,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="119" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50093,7 +50132,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="124" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -50151,7 +50190,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="125" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B3" s="126">
         <v>45596.0</v>
@@ -50444,261 +50483,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="129" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B4" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C4" s="131" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="132" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="132" t="s">
-        <v>186</v>
-      </c>
       <c r="E4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O4" s="132" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P4" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U4" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE4" s="134" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AI4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AJ4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL4" s="134" t="s">
+        <v>192</v>
+      </c>
+      <c r="AM4" s="132" t="s">
         <v>190</v>
       </c>
-      <c r="AF4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AH4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK4" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="AL4" s="134" t="s">
-        <v>191</v>
-      </c>
-      <c r="AM4" s="132" t="s">
-        <v>189</v>
-      </c>
       <c r="AN4" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP4" s="134" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AQ4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS4" s="134" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AT4" s="135" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AV4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY4" s="134" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AZ4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI4" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ4" s="134" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="BK4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BL4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BM4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BN4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BO4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BP4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BQ4" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BR4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CD4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG4" s="132"/>
       <c r="CH4" s="132"/>
       <c r="CI4" s="134" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="CJ4" s="132"/>
       <c r="CK4" s="132"/>
@@ -50710,249 +50749,249 @@
       <c r="CQ4" s="132"/>
       <c r="CR4" s="132"/>
       <c r="CS4" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="129" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P5" s="133" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Q5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U5" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="V5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE5" s="136"/>
       <c r="AF5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL5" s="136"/>
       <c r="AM5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP5" s="136"/>
       <c r="AQ5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AR5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AS5" s="136"/>
       <c r="AT5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AU5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AV5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AW5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AX5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AY5" s="136"/>
       <c r="AZ5" s="132" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="BA5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI5" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ5" s="136"/>
       <c r="BK5" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL5" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN5" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BP5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CD5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG5" s="132"/>
       <c r="CH5" s="132"/>
@@ -50967,249 +51006,249 @@
       <c r="CQ5" s="132"/>
       <c r="CR5" s="132"/>
       <c r="CS5" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="129" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B6" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K6" s="137" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O6" s="132" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="V6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE6" s="136"/>
       <c r="AF6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL6" s="136"/>
       <c r="AM6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP6" s="136"/>
       <c r="AQ6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS6" s="136"/>
       <c r="AT6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AV6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY6" s="136"/>
       <c r="AZ6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ6" s="136"/>
       <c r="BK6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM6" s="132" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="BN6" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BP6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CD6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG6" s="132"/>
       <c r="CH6" s="132"/>
@@ -51224,198 +51263,198 @@
       <c r="CQ6" s="132"/>
       <c r="CR6" s="132"/>
       <c r="CS6" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="129" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B7" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L7" s="137" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O7" s="132" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P7" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U7" s="133" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="V7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z7" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE7" s="136"/>
       <c r="AF7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL7" s="136"/>
       <c r="AM7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP7" s="136"/>
       <c r="AQ7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS7" s="136"/>
       <c r="AT7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU7" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AV7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY7" s="136"/>
       <c r="AZ7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI7" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ7" s="136"/>
       <c r="BK7" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL7" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN7" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO7" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BP7" s="132"/>
       <c r="BQ7" s="132"/>
@@ -51423,16 +51462,16 @@
       <c r="BS7" s="132"/>
       <c r="BT7" s="132"/>
       <c r="BU7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX7" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY7" s="132"/>
       <c r="BZ7" s="132"/>
@@ -51458,220 +51497,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="129" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B8" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L8" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="M8" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="O8" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="M8" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="N8" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="O8" s="132" t="s">
-        <v>188</v>
-      </c>
       <c r="P8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="V8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W8" s="132" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="X8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB8" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE8" s="136"/>
       <c r="AF8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL8" s="136"/>
       <c r="AM8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN8" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP8" s="136"/>
       <c r="AQ8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS8" s="136"/>
       <c r="AT8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AV8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY8" s="136"/>
       <c r="AZ8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG8" s="132" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="BH8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ8" s="136"/>
       <c r="BK8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN8" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BP8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW8" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX8" s="132" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BY8" s="132"/>
       <c r="BZ8" s="132"/>
@@ -51697,244 +51736,244 @@
     </row>
     <row r="9">
       <c r="A9" s="129" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B9" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O9" s="137" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="V9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE9" s="136"/>
       <c r="AF9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL9" s="136"/>
       <c r="AM9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP9" s="136"/>
       <c r="AQ9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS9" s="136"/>
       <c r="AT9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AV9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY9" s="136"/>
       <c r="AZ9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ9" s="136"/>
       <c r="BK9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN9" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BP9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CD9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG9" s="132"/>
       <c r="CH9" s="132"/>
@@ -51949,249 +51988,249 @@
       <c r="CQ9" s="132"/>
       <c r="CR9" s="132"/>
       <c r="CS9" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="129" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B10" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I10" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="J10" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="K10" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="L10" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="M10" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="N10" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="O10" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="J10" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="K10" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="L10" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="M10" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="N10" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="O10" s="132" t="s">
-        <v>188</v>
-      </c>
       <c r="P10" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Q10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U10" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AE10" s="136"/>
       <c r="AF10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AL10" s="136"/>
       <c r="AM10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AN10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP10" s="136"/>
       <c r="AQ10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS10" s="136"/>
       <c r="AT10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AV10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY10" s="136"/>
       <c r="AZ10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BA10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BB10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BC10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BD10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BE10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BF10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BG10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BH10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI10" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ10" s="136"/>
       <c r="BK10" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL10" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN10" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BP10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW10" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BX10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CD10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG10" s="132"/>
       <c r="CH10" s="132"/>
@@ -52206,249 +52245,249 @@
       <c r="CQ10" s="132"/>
       <c r="CR10" s="132"/>
       <c r="CS10" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="129" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B11" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J11" s="132" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K11" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="L11" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="M11" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="N11" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="O11" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="L11" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="M11" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="N11" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="O11" s="132" t="s">
-        <v>188</v>
-      </c>
       <c r="P11" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="T11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U11" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Y11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Z11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AB11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AC11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AE11" s="136"/>
       <c r="AF11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AI11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL11" s="136"/>
       <c r="AM11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP11" s="136"/>
       <c r="AQ11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AR11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AS11" s="136"/>
       <c r="AT11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AU11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AV11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AW11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AY11" s="136"/>
       <c r="AZ11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BA11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BB11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BC11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BE11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BF11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BG11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BH11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI11" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BJ11" s="136"/>
       <c r="BK11" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BL11" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BM11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN11" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BO11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BP11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BQ11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BR11" s="132" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="BS11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BT11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BU11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BX11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BY11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CA11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CC11" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CD11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG11" s="132"/>
       <c r="CH11" s="132"/>
@@ -52463,249 +52502,249 @@
       <c r="CQ11" s="132"/>
       <c r="CR11" s="132"/>
       <c r="CS11" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="129" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B12" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="H12" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="L12" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="M12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="N12" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="O12" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="E12" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="F12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="H12" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="I12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="J12" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="K12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="L12" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="M12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="N12" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="O12" s="132" t="s">
-        <v>188</v>
-      </c>
       <c r="P12" s="133" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="S12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="T12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U12" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="W12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Y12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Z12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AB12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AE12" s="136"/>
       <c r="AF12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AG12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AH12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AI12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AJ12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AL12" s="136"/>
       <c r="AM12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AN12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AP12" s="136"/>
       <c r="AQ12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AR12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AS12" s="136"/>
       <c r="AT12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AU12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AV12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AX12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AY12" s="136"/>
       <c r="AZ12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BA12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BB12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BC12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BD12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BE12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BF12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BG12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BH12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BI12" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BJ12" s="136"/>
       <c r="BK12" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BL12" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BM12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BN12" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BO12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BP12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BQ12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BR12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BS12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BT12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BU12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BV12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BW12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BX12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BY12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="BZ12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CA12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CB12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CC12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CD12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CE12" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CG12" s="132"/>
       <c r="CH12" s="132"/>
@@ -52720,249 +52759,249 @@
       <c r="CQ12" s="132"/>
       <c r="CR12" s="132"/>
       <c r="CS12" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="129" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B13" s="130" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="G13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="J13" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="K13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="L13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="M13" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="N13" s="132" t="s">
+        <v>190</v>
+      </c>
+      <c r="O13" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="E13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="F13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="G13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="H13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="J13" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="K13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="L13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="M13" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="N13" s="132" t="s">
-        <v>189</v>
-      </c>
-      <c r="O13" s="132" t="s">
-        <v>188</v>
-      </c>
       <c r="P13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Q13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="S13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="T13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="X13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Y13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Z13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AB13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AD13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AE13" s="138"/>
       <c r="AF13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AG13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AH13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AI13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AK13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AL13" s="138"/>
       <c r="AM13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AN13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AP13" s="138"/>
       <c r="AQ13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AR13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AS13" s="138"/>
       <c r="AT13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AU13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AV13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AW13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AX13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AY13" s="138"/>
       <c r="AZ13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BA13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BB13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BC13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BD13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BE13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BF13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BG13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BH13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BI13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BJ13" s="138"/>
       <c r="BK13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BL13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BM13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BN13" s="133" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BO13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BP13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BQ13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BR13" s="132" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="BS13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BT13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BU13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BV13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BW13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BX13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BY13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="BZ13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CA13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CB13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CC13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CD13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CE13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CF13" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CG13" s="132"/>
       <c r="CH13" s="132"/>
@@ -52977,7 +53016,7 @@
       <c r="CQ13" s="132"/>
       <c r="CR13" s="132"/>
       <c r="CS13" s="132" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54003,7 +54042,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="139" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="139" t="s">
         <v>2</v>
@@ -54030,13 +54069,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="143" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K1" s="144" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L1" s="142" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M1" s="145"/>
       <c r="N1" s="145"/>
@@ -54055,10 +54094,10 @@
     </row>
     <row r="2">
       <c r="A2" s="146" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="147" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148" t="s">
@@ -54085,7 +54124,7 @@
       </c>
       <c r="K2" s="151"/>
       <c r="L2" s="152" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M2" s="145"/>
       <c r="N2" s="145"/>
@@ -54104,13 +54143,13 @@
     </row>
     <row r="3">
       <c r="A3" s="146" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B3" s="153" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C3" s="154" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D3" s="148" t="s">
         <v>39</v>
@@ -54132,7 +54171,7 @@
       </c>
       <c r="K3" s="149"/>
       <c r="L3" s="152" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M3" s="155"/>
       <c r="N3" s="145"/>
@@ -54151,11 +54190,11 @@
     </row>
     <row r="4">
       <c r="A4" s="146" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B4" s="136"/>
       <c r="C4" s="156" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D4" s="148" t="s">
         <v>39</v>
@@ -54177,7 +54216,7 @@
       </c>
       <c r="K4" s="157"/>
       <c r="L4" s="160" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M4" s="155"/>
       <c r="N4" s="145"/>
@@ -54196,13 +54235,13 @@
     </row>
     <row r="5">
       <c r="A5" s="146" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B5" s="142" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C5" s="148" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D5" s="148" t="s">
         <v>39</v>
@@ -54224,7 +54263,7 @@
       </c>
       <c r="K5" s="149"/>
       <c r="L5" s="152" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M5" s="155"/>
       <c r="N5" s="145"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 22  de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_Colmedica.xlsx
+++ b/Segumiento_Colmedica.xlsx
@@ -2752,7 +2752,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32785</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2814,7 +2814,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="24">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32785</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -3098,7 +3098,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3376,7 +3376,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32785</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3802,7 +3802,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3942,7 +3942,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4072,7 +4072,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32785</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="18" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
@@ -4200,7 +4200,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>32784</v>
+        <v>32785</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4249,7 +4249,7 @@
         <v>20</v>
       </c>
       <c r="G29" s="34">
-        <v>60.0</v>
+        <v>100.0</v>
       </c>
       <c r="H29" s="35">
         <v>2.0</v>
@@ -4260,7 +4260,9 @@
       <c r="J29" s="37">
         <v>45917.0</v>
       </c>
-      <c r="K29" s="38"/>
+      <c r="K29" s="38">
+        <v>45918.0</v>
+      </c>
       <c r="L29" s="38">
         <v>45918.0</v>
       </c>
@@ -4321,7 +4323,7 @@
         <v>20</v>
       </c>
       <c r="G30" s="19">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="H30" s="20">
         <v>3.0</v>
@@ -4408,7 +4410,7 @@
       <c r="L31" s="38"/>
       <c r="M31" s="39">
         <f>IF(ISBLANK(L31), NETWORKDAYS(J31, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J31, L31, Hoja2!$A$1:$A$18))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N31" s="38"/>
       <c r="O31" s="38"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 29  de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_Colmedica.xlsx
+++ b/Segumiento_Colmedica.xlsx
@@ -10,7 +10,7 @@
     <sheet state="hidden" name="pruebas i" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$33</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$34</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'PRUEBAS BOLIVAR'!$A$1:$L$16</definedName>
   </definedNames>
   <calcPr/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="235">
   <si>
     <t>Asignado a</t>
   </si>
@@ -556,10 +556,19 @@
     <t>OPT_14</t>
   </si>
   <si>
-    <t>Afiliaciones Pre - Sarlaft derivado del REQ-303</t>
+    <t>Afiliaciones Pre - Sarlaft derivado del REQ-313</t>
   </si>
   <si>
     <t>validar cantidades del excel vs los pdf, cambiar el renombre de los archivos tomando como base el excel e ir a buscar la cc en el nombre del archivo y así asignarle la solicitud, al final imprima mensaje indicando si algo quedó en estado 1 o estado 2 "Quedaron solicitudes en estado pendiente" - "Todo procesado correctamente"</t>
+  </si>
+  <si>
+    <t>25/09/2025 Se valida el funcionamiento del script encargado y su proceso corresponde a la descripcion del req</t>
+  </si>
+  <si>
+    <t>Acreditación - Consulta Puntual en BDEX</t>
+  </si>
+  <si>
+    <t>Consulta de usuarios en régimen especial, de manera automática en página del Adres. se necesita homologar logueo con usuario y contraseña, y al momento de la consulta de cada identificación revisar el captchap que se muestra. generar consultas en intervalo de tiempos para no generar algun tipo de laerta, dado que se usan logueos del cliente</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2785,7 +2794,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32788</v>
+        <v>32790</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2847,7 +2856,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="24">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>32788</v>
+        <v>32790</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -3131,7 +3140,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3409,7 +3418,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32788</v>
+        <v>32790</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3835,7 +3844,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3975,7 +3984,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4105,7 +4114,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32788</v>
+        <v>32790</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4243,7 +4252,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4570,7 +4579,7 @@
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="33" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="G33" s="34">
         <v>10.0</v>
@@ -4584,12 +4593,24 @@
       <c r="J33" s="37">
         <v>45925.0</v>
       </c>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="40"/>
+      <c r="K33" s="37">
+        <v>45925.0</v>
+      </c>
+      <c r="L33" s="37">
+        <v>45925.0</v>
+      </c>
+      <c r="M33" s="37">
+        <v>45925.0</v>
+      </c>
+      <c r="N33" s="37">
+        <v>45925.0</v>
+      </c>
+      <c r="O33" s="37">
+        <v>45925.0</v>
+      </c>
+      <c r="P33" s="40" t="s">
+        <v>133</v>
+      </c>
       <c r="Q33" s="41" t="b">
         <v>1</v>
       </c>
@@ -4619,13 +4640,21 @@
     <row r="34">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>135</v>
+      </c>
       <c r="E34" s="17"/>
-      <c r="F34" s="18"/>
+      <c r="F34" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="G34" s="19"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="21"/>
+      <c r="I34" s="21">
+        <v>45929.0</v>
+      </c>
       <c r="J34" s="22"/>
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
@@ -4633,7 +4662,9 @@
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
       <c r="P34" s="25"/>
-      <c r="Q34" s="26"/>
+      <c r="Q34" s="26" t="b">
+        <v>0</v>
+      </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
       <c r="T34" s="27"/>
@@ -41804,7 +41835,7 @@
       <c r="AM940" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Q$33"/>
+  <autoFilter ref="$A$1:$Q$34"/>
   <conditionalFormatting sqref="B2:B42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(B$2:B$16,B2)&gt;1</formula>
@@ -41814,7 +41845,7 @@
     <dataValidation type="list" allowBlank="1" sqref="F2:F940">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:O26 I27 I28:L940 N28:O940">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:O26 I27 I28:L32 N28:O32 I33:O33 I34:L940 N34:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -41853,7 +41884,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="85" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>2</v>
@@ -41880,13 +41911,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="88" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K1" s="85" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L1" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M1" s="90"/>
       <c r="N1" s="90"/>
@@ -41905,14 +41936,14 @@
     </row>
     <row r="2">
       <c r="A2" s="91" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2" s="93"/>
       <c r="D2" s="94" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E2" s="95">
         <v>45526.0</v>
@@ -41926,7 +41957,7 @@
       <c r="J2" s="93"/>
       <c r="K2" s="93"/>
       <c r="L2" s="93" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="M2" s="96"/>
       <c r="N2" s="96"/>
@@ -41945,13 +41976,13 @@
     </row>
     <row r="3">
       <c r="A3" s="97" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B3" s="98" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D3" s="99" t="s">
         <v>20</v>
@@ -41975,7 +42006,7 @@
       </c>
       <c r="K3" s="101"/>
       <c r="L3" s="103" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M3" s="90"/>
       <c r="N3" s="90"/>
@@ -41994,16 +42025,16 @@
     </row>
     <row r="4">
       <c r="A4" s="104" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C4" s="104" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D4" s="106" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E4" s="107">
         <v>45581.0</v>
@@ -42026,7 +42057,7 @@
       </c>
       <c r="K4" s="107"/>
       <c r="L4" s="104" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="M4" s="110"/>
       <c r="N4" s="110"/>
@@ -42045,16 +42076,16 @@
     </row>
     <row r="5">
       <c r="A5" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D5" s="111" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E5" s="100">
         <v>45572.0</v>
@@ -42075,7 +42106,7 @@
       </c>
       <c r="K5" s="100"/>
       <c r="L5" s="103" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="M5" s="90"/>
       <c r="N5" s="90"/>
@@ -42094,16 +42125,16 @@
     </row>
     <row r="6">
       <c r="A6" s="112" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B6" s="112" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E6" s="113">
         <v>45602.0</v>
@@ -42124,7 +42155,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="114" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M6" s="115"/>
       <c r="N6" s="116"/>
@@ -42143,16 +42174,16 @@
     </row>
     <row r="7">
       <c r="A7" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C7" s="117" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D7" s="111" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E7" s="100">
         <v>45589.0</v>
@@ -42173,7 +42204,7 @@
       </c>
       <c r="K7" s="111"/>
       <c r="L7" s="119" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="M7" s="120"/>
       <c r="N7" s="120"/>
@@ -42192,14 +42223,14 @@
     </row>
     <row r="8">
       <c r="A8" s="121" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B8" s="122" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C8" s="123"/>
       <c r="D8" s="123" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E8" s="124">
         <v>45603.0</v>
@@ -42220,7 +42251,7 @@
       </c>
       <c r="K8" s="124"/>
       <c r="L8" s="126" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="M8" s="90"/>
       <c r="N8" s="90"/>
@@ -42239,16 +42270,16 @@
     </row>
     <row r="9">
       <c r="A9" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B9" s="128" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C9" s="129" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E9" s="131">
         <v>45671.0</v>
@@ -42257,7 +42288,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="129" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H9" s="131">
         <v>45680.0</v>
@@ -42271,7 +42302,7 @@
       </c>
       <c r="K9" s="129"/>
       <c r="L9" s="133" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M9" s="134"/>
       <c r="N9" s="134"/>
@@ -42290,14 +42321,14 @@
     </row>
     <row r="10">
       <c r="A10" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B10" s="135"/>
       <c r="C10" s="133" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="130" t="s">
         <v>169</v>
-      </c>
-      <c r="D10" s="130" t="s">
-        <v>166</v>
       </c>
       <c r="E10" s="131">
         <v>45671.0</v>
@@ -42316,7 +42347,7 @@
       <c r="J10" s="129"/>
       <c r="K10" s="129"/>
       <c r="L10" s="133" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="M10" s="134"/>
       <c r="N10" s="134"/>
@@ -42335,14 +42366,14 @@
     </row>
     <row r="11">
       <c r="A11" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B11" s="135"/>
       <c r="C11" s="133" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E11" s="131">
         <v>45671.0</v>
@@ -42361,7 +42392,7 @@
       <c r="J11" s="129"/>
       <c r="K11" s="129"/>
       <c r="L11" s="133" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="M11" s="134"/>
       <c r="N11" s="134"/>
@@ -42380,14 +42411,14 @@
     </row>
     <row r="12">
       <c r="A12" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B12" s="135"/>
       <c r="C12" s="133" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D12" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E12" s="131">
         <v>45671.0</v>
@@ -42406,7 +42437,7 @@
       <c r="J12" s="129"/>
       <c r="K12" s="129"/>
       <c r="L12" s="133" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="M12" s="134"/>
       <c r="N12" s="134"/>
@@ -42425,14 +42456,14 @@
     </row>
     <row r="13">
       <c r="A13" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B13" s="135"/>
       <c r="C13" s="133" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D13" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E13" s="131">
         <v>45671.0</v>
@@ -42451,7 +42482,7 @@
       <c r="J13" s="129"/>
       <c r="K13" s="129"/>
       <c r="L13" s="133" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="M13" s="134"/>
       <c r="N13" s="134"/>
@@ -42470,14 +42501,14 @@
     </row>
     <row r="14">
       <c r="A14" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B14" s="135"/>
       <c r="C14" s="133" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D14" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E14" s="131">
         <v>45671.0</v>
@@ -42496,7 +42527,7 @@
       <c r="J14" s="129"/>
       <c r="K14" s="129"/>
       <c r="L14" s="129" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="M14" s="134"/>
       <c r="N14" s="134"/>
@@ -42515,14 +42546,14 @@
     </row>
     <row r="15">
       <c r="A15" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B15" s="135"/>
       <c r="C15" s="133" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D15" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E15" s="131">
         <v>45671.0</v>
@@ -42541,7 +42572,7 @@
       <c r="J15" s="129"/>
       <c r="K15" s="129"/>
       <c r="L15" s="129" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="M15" s="134"/>
       <c r="N15" s="134"/>
@@ -42560,14 +42591,14 @@
     </row>
     <row r="16">
       <c r="A16" s="127" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B16" s="136"/>
       <c r="C16" s="137" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D16" s="130" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E16" s="131">
         <v>45681.0</v>
@@ -42586,7 +42617,7 @@
       <c r="J16" s="129"/>
       <c r="K16" s="129"/>
       <c r="L16" s="133" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="M16" s="134"/>
       <c r="N16" s="134"/>
@@ -49122,7 +49153,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="134" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49130,7 +49161,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49138,7 +49169,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="134" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49146,7 +49177,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="134" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49154,7 +49185,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="134" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49162,7 +49193,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="134" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49170,7 +49201,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="134" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49178,7 +49209,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="134" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49186,7 +49217,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="134" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49194,7 +49225,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="134" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49202,7 +49233,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="134" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49210,7 +49241,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="134" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49218,7 +49249,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="134" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49226,7 +49257,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="134" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49234,7 +49265,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="134" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49242,7 +49273,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="134" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49250,7 +49281,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="134" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49258,7 +49289,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="134" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50274,7 +50305,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="139" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B1" s="134"/>
       <c r="C1" s="134"/>
@@ -50332,7 +50363,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="140" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B3" s="141">
         <v>45596.0</v>
@@ -50625,261 +50656,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="144" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B4" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C4" s="146" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="M4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O4" s="147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="P4" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U4" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="V4" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="V4" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="W4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE4" s="149" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="AF4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL4" s="149" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="AM4" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN4" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO4" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AN4" s="147" t="s">
+      <c r="AP4" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="AQ4" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AO4" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="AP4" s="149" t="s">
-        <v>205</v>
-      </c>
-      <c r="AQ4" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AR4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS4" s="149" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AT4" s="150" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AV4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AW4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY4" s="149" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AZ4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BH4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI4" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ4" s="149" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="BK4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BL4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BM4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BN4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BO4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BP4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BQ4" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BR4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CC4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CD4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CF4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG4" s="147"/>
       <c r="CH4" s="147"/>
       <c r="CI4" s="149" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="CJ4" s="147"/>
       <c r="CK4" s="147"/>
@@ -50891,249 +50922,249 @@
       <c r="CQ4" s="147"/>
       <c r="CR4" s="147"/>
       <c r="CS4" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="144" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B5" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="N5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="O5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="P5" s="148" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Q5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U5" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="V5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE5" s="151"/>
       <c r="AF5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL5" s="151"/>
       <c r="AM5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AO5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP5" s="151"/>
       <c r="AQ5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AR5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AS5" s="151"/>
       <c r="AT5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AU5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AV5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AW5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AX5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AY5" s="151"/>
       <c r="AZ5" s="147" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="BA5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BH5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI5" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ5" s="151"/>
       <c r="BK5" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL5" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN5" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BP5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BQ5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CC5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CD5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CF5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG5" s="147"/>
       <c r="CH5" s="147"/>
@@ -51148,249 +51179,249 @@
       <c r="CQ5" s="147"/>
       <c r="CR5" s="147"/>
       <c r="CS5" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="144" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B6" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K6" s="152" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="L6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="M6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O6" s="147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="P6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="V6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE6" s="151"/>
       <c r="AF6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL6" s="151"/>
       <c r="AM6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AO6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP6" s="151"/>
       <c r="AQ6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS6" s="151"/>
       <c r="AT6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AV6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AW6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY6" s="151"/>
       <c r="AZ6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BH6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ6" s="151"/>
       <c r="BK6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM6" s="147" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="BN6" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BP6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BQ6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CC6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CD6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CF6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG6" s="147"/>
       <c r="CH6" s="147"/>
@@ -51405,198 +51436,198 @@
       <c r="CQ6" s="147"/>
       <c r="CR6" s="147"/>
       <c r="CS6" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="144" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B7" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L7" s="152" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="M7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O7" s="147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="P7" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U7" s="148" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="V7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z7" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA7" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AA7" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AB7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE7" s="151"/>
       <c r="AF7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL7" s="151"/>
       <c r="AM7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AO7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP7" s="151"/>
       <c r="AQ7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS7" s="151"/>
       <c r="AT7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU7" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AV7" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AV7" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AW7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY7" s="151"/>
       <c r="AZ7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BH7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI7" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ7" s="151"/>
       <c r="BK7" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL7" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN7" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO7" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BP7" s="147"/>
       <c r="BQ7" s="147"/>
@@ -51604,16 +51635,16 @@
       <c r="BS7" s="147"/>
       <c r="BT7" s="147"/>
       <c r="BU7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX7" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY7" s="147"/>
       <c r="BZ7" s="147"/>
@@ -51639,220 +51670,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="144" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B8" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L8" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="M8" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="M8" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="N8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O8" s="147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="P8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="V8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W8" s="147" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="X8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB8" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC8" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AC8" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AD8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE8" s="151"/>
       <c r="AF8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL8" s="151"/>
       <c r="AM8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN8" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO8" s="147" t="s">
         <v>202</v>
-      </c>
-      <c r="AO8" s="147" t="s">
-        <v>199</v>
       </c>
       <c r="AP8" s="151"/>
       <c r="AQ8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS8" s="151"/>
       <c r="AT8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AV8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AW8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY8" s="151"/>
       <c r="AZ8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG8" s="147" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="BH8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ8" s="151"/>
       <c r="BK8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN8" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BP8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BQ8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW8" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX8" s="147" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="BY8" s="147"/>
       <c r="BZ8" s="147"/>
@@ -51878,244 +51909,244 @@
     </row>
     <row r="9">
       <c r="A9" s="144" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B9" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="M9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="O9" s="152" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="P9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="U9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="V9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE9" s="151"/>
       <c r="AF9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL9" s="151"/>
       <c r="AM9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AO9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP9" s="151"/>
       <c r="AQ9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS9" s="151"/>
       <c r="AT9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AV9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AW9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY9" s="151"/>
       <c r="AZ9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BB9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BF9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BG9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BH9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BI9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BJ9" s="151"/>
       <c r="BK9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN9" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BP9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BQ9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CC9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CD9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CF9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG9" s="147"/>
       <c r="CH9" s="147"/>
@@ -52130,249 +52161,249 @@
       <c r="CQ9" s="147"/>
       <c r="CR9" s="147"/>
       <c r="CS9" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="144" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B10" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="J10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="J10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="K10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="L10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="L10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="M10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="O10" s="147" t="s">
+        <v>204</v>
+      </c>
+      <c r="P10" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="R10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="O10" s="147" t="s">
-        <v>201</v>
-      </c>
-      <c r="P10" s="148" t="s">
+      <c r="S10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="Q10" s="147" t="s">
+      <c r="T10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="R10" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="S10" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="T10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="U10" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="V10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="V10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="W10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="X10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Y10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AE10" s="151"/>
       <c r="AF10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK10" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AL10" s="151"/>
       <c r="AM10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AN10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AO10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP10" s="151"/>
       <c r="AQ10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS10" s="151"/>
       <c r="AT10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AV10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AW10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AX10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AY10" s="151"/>
       <c r="AZ10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BA10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BD10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BB10" s="147" t="s">
+      <c r="BG10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BC10" s="147" t="s">
+      <c r="BH10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BD10" s="147" t="s">
+      <c r="BI10" s="148" t="s">
         <v>202</v>
-      </c>
-      <c r="BE10" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BF10" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BG10" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BH10" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BI10" s="148" t="s">
-        <v>199</v>
       </c>
       <c r="BJ10" s="151"/>
       <c r="BK10" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL10" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN10" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BP10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BQ10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BS10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW10" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BX10" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BX10" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="BY10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CC10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CD10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CF10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG10" s="147"/>
       <c r="CH10" s="147"/>
@@ -52387,249 +52418,249 @@
       <c r="CQ10" s="147"/>
       <c r="CR10" s="147"/>
       <c r="CS10" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="144" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B11" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J11" s="147" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="K11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="L11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="L11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="M11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="N11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="N11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="O11" s="147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="P11" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="T11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="U11" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="V11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="T11" s="147" t="s">
+      <c r="W11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="U11" s="148" t="s">
+      <c r="X11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="V11" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="W11" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="X11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="Y11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Z11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AB11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AC11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AD11" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AE11" s="151"/>
       <c r="AF11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AG11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AH11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AI11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AJ11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AK11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AL11" s="151"/>
       <c r="AM11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AN11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AO11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AP11" s="151"/>
       <c r="AQ11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AR11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AS11" s="151"/>
       <c r="AT11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AU11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AV11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AV11" s="147" t="s">
+      <c r="AX11" s="147" t="s">
         <v>202</v>
-      </c>
-      <c r="AW11" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="AX11" s="147" t="s">
-        <v>199</v>
       </c>
       <c r="AY11" s="151"/>
       <c r="AZ11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BA11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="BB11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BC11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BD11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BE11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BG11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BF11" s="147" t="s">
+      <c r="BI11" s="148" t="s">
         <v>202</v>
-      </c>
-      <c r="BG11" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BH11" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BI11" s="148" t="s">
-        <v>199</v>
       </c>
       <c r="BJ11" s="151"/>
       <c r="BK11" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BL11" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BM11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BN11" s="148" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BO11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BP11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="BQ11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BR11" s="147" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="BS11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BT11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BU11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BV11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BW11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BX11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BY11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="BZ11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CA11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CB11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CC11" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CD11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="CC11" s="147" t="s">
+      <c r="CE11" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="CD11" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="CE11" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="CF11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CG11" s="147"/>
       <c r="CH11" s="147"/>
@@ -52644,249 +52675,249 @@
       <c r="CQ11" s="147"/>
       <c r="CR11" s="147"/>
       <c r="CS11" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="144" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B12" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="E12" s="147" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="G12" s="147" t="s">
+      <c r="I12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="J12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="I12" s="147" t="s">
+      <c r="K12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="L12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="J12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="K12" s="147" t="s">
+      <c r="M12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="N12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="O12" s="147" t="s">
+        <v>204</v>
+      </c>
+      <c r="P12" s="148" t="s">
         <v>202</v>
       </c>
-      <c r="L12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="M12" s="147" t="s">
+      <c r="Q12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="R12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="S12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="T12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="U12" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="V12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="W12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="N12" s="147" t="s">
+      <c r="X12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="O12" s="147" t="s">
-        <v>201</v>
-      </c>
-      <c r="P12" s="148" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q12" s="147" t="s">
+      <c r="AA12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="R12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="S12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="T12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="U12" s="148" t="s">
-        <v>202</v>
-      </c>
-      <c r="V12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="W12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="X12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="Y12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="AA12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC12" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AD12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AE12" s="151"/>
       <c r="AF12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AG12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AG12" s="147" t="s">
+      <c r="AK12" s="147" t="s">
         <v>202</v>
-      </c>
-      <c r="AH12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AI12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="AK12" s="147" t="s">
-        <v>199</v>
       </c>
       <c r="AL12" s="151"/>
       <c r="AM12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AN12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AO12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AP12" s="151"/>
       <c r="AQ12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AR12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AS12" s="151"/>
       <c r="AT12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AV12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AU12" s="147" t="s">
+      <c r="AW12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AV12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW12" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AX12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AY12" s="151"/>
       <c r="AZ12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BA12" s="147" t="s">
+      <c r="BD12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BB12" s="147" t="s">
+      <c r="BF12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BG12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BC12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BD12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BE12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BF12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BG12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BH12" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="BI12" s="148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BJ12" s="151"/>
       <c r="BK12" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL12" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BM12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BL12" s="148" t="s">
+      <c r="BN12" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BQ12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BR12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BM12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BN12" s="148" t="s">
+      <c r="BS12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BT12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BU12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BO12" s="147" t="s">
+      <c r="BV12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BP12" s="147" t="s">
+      <c r="BW12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BX12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BY12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BQ12" s="147" t="s">
+      <c r="BZ12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CA12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CB12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BR12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BS12" s="147" t="s">
+      <c r="CC12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CD12" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CE12" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BT12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BU12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BV12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BW12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BX12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BY12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="BZ12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CA12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CB12" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="CC12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CD12" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CE12" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="CF12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CG12" s="147"/>
       <c r="CH12" s="147"/>
@@ -52901,249 +52932,249 @@
       <c r="CQ12" s="147"/>
       <c r="CR12" s="147"/>
       <c r="CS12" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="144" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B13" s="145" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="H13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="J13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="D13" s="147" t="s">
+      <c r="K13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="L13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="M13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="E13" s="147" t="s">
+      <c r="N13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="O13" s="147" t="s">
+        <v>204</v>
+      </c>
+      <c r="P13" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="R13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="S13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="T13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="U13" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="V13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="F13" s="147" t="s">
+      <c r="W13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="X13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="G13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="H13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="I13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="J13" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="K13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="L13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="M13" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="N13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="O13" s="147" t="s">
-        <v>201</v>
-      </c>
-      <c r="P13" s="148" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="R13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="S13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="T13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="U13" s="148" t="s">
-        <v>202</v>
-      </c>
-      <c r="V13" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="W13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="X13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="Y13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AA13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC13" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AD13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AE13" s="153"/>
       <c r="AF13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AG13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="AG13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="AI13" s="147" t="s">
-        <v>199</v>
-      </c>
       <c r="AJ13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AK13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AL13" s="153"/>
       <c r="AM13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AN13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AO13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AP13" s="153"/>
       <c r="AQ13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AR13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AS13" s="153"/>
       <c r="AT13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AU13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AV13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AW13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AX13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AY13" s="153"/>
       <c r="AZ13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BA13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BB13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BC13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BD13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BE13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BF13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BG13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BH13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BI13" s="148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BJ13" s="153"/>
       <c r="BK13" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL13" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BM13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BN13" s="148" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BQ13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BR13" s="147" t="s">
+        <v>223</v>
+      </c>
+      <c r="BS13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BT13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BU13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BV13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BW13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BX13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BY13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="BZ13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CA13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CB13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CC13" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="CD13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BL13" s="148" t="s">
+      <c r="CE13" s="147" t="s">
         <v>202</v>
       </c>
-      <c r="BM13" s="147" t="s">
+      <c r="CF13" s="147" t="s">
         <v>202</v>
-      </c>
-      <c r="BN13" s="148" t="s">
-        <v>202</v>
-      </c>
-      <c r="BO13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BP13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BQ13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BR13" s="147" t="s">
-        <v>220</v>
-      </c>
-      <c r="BS13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BT13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BU13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BV13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BW13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BX13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BY13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BZ13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CA13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CB13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CC13" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="CD13" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="CE13" s="147" t="s">
-        <v>199</v>
-      </c>
-      <c r="CF13" s="147" t="s">
-        <v>199</v>
       </c>
       <c r="CG13" s="147"/>
       <c r="CH13" s="147"/>
@@ -53158,7 +53189,7 @@
       <c r="CQ13" s="147"/>
       <c r="CR13" s="147"/>
       <c r="CS13" s="147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54184,7 +54215,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="154" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B1" s="154" t="s">
         <v>2</v>
@@ -54211,13 +54242,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="158" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K1" s="159" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L1" s="157" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M1" s="160"/>
       <c r="N1" s="160"/>
@@ -54236,10 +54267,10 @@
     </row>
     <row r="2">
       <c r="A2" s="161" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B2" s="162" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C2" s="163"/>
       <c r="D2" s="163" t="s">
@@ -54266,7 +54297,7 @@
       </c>
       <c r="K2" s="166"/>
       <c r="L2" s="167" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="M2" s="160"/>
       <c r="N2" s="160"/>
@@ -54285,13 +54316,13 @@
     </row>
     <row r="3">
       <c r="A3" s="161" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C3" s="169" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D3" s="163" t="s">
         <v>39</v>
@@ -54313,7 +54344,7 @@
       </c>
       <c r="K3" s="164"/>
       <c r="L3" s="167" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="M3" s="170"/>
       <c r="N3" s="160"/>
@@ -54332,11 +54363,11 @@
     </row>
     <row r="4">
       <c r="A4" s="161" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B4" s="151"/>
       <c r="C4" s="171" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D4" s="163" t="s">
         <v>39</v>
@@ -54358,7 +54389,7 @@
       </c>
       <c r="K4" s="172"/>
       <c r="L4" s="175" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="M4" s="170"/>
       <c r="N4" s="160"/>
@@ -54377,13 +54408,13 @@
     </row>
     <row r="5">
       <c r="A5" s="161" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B5" s="157" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C5" s="163" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D5" s="163" t="s">
         <v>39</v>
@@ -54405,7 +54436,7 @@
       </c>
       <c r="K5" s="164"/>
       <c r="L5" s="167" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="M5" s="170"/>
       <c r="N5" s="160"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 01 de octubre
</commit_message>
<xml_diff>
--- a/Segumiento_Colmedica.xlsx
+++ b/Segumiento_Colmedica.xlsx
@@ -10,7 +10,7 @@
     <sheet state="hidden" name="pruebas i" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$34</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$35</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'PRUEBAS BOLIVAR'!$A$1:$L$16</definedName>
   </definedNames>
   <calcPr/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="242">
   <si>
     <t>Asignado a</t>
   </si>
@@ -475,6 +475,9 @@
 08/09/2025 Se realiza ajuste en backend y frontend para reestabecer la contraseña</t>
   </si>
   <si>
+    <t>JOHN</t>
+  </si>
+  <si>
     <t>OPT_10</t>
   </si>
   <si>
@@ -550,7 +553,12 @@
     <t>Consolidados Pendientes Proceso - Estados UMD</t>
   </si>
   <si>
-    <t>23/09/2025 Se inicia con la identificación de lo que se desea mostrar, primera imagens seguimiento del periodo en curso con estados, valores y cantidades</t>
+    <t>Crear graficas de la produccion del proceso actual, para mostrar estados, valores</t>
+  </si>
+  <si>
+    <t>23/09/2025 Se inicia con la identificación de lo que se desea mostrar, primera imagens seguimiento del periodo en curso con estados, valores y cantidades
+25/09/2025 se termina de ajustar la grafica para mostrar proceso actual, estados y los valores correspondientes. Se dispone en ambiente de pruebas para revisar que funciona de manera correcta.
+26/09/2025 se pasa a produccion las páginas realizadas y se deja disponible para la visualizacion tanto del área operativa como del cliente</t>
   </si>
   <si>
     <t>OPT_14</t>
@@ -568,7 +576,28 @@
     <t>Acreditación - Consulta Puntual en BDEX</t>
   </si>
   <si>
-    <t>Consulta de usuarios en régimen especial, de manera automática en página del Adres. se necesita homologar logueo con usuario y contraseña, y al momento de la consulta de cada identificación revisar el captchap que se muestra. generar consultas en intervalo de tiempos para no generar algun tipo de laerta, dado que se usan logueos del cliente</t>
+    <t>Consulta de usuarios en régimen especial los pendinetes por acreditar de las vigencias activas para revisar, de manera automática en página del Adres. se necesita homologar logueo con usuario y contraseña, y al momento de la consulta de cada identificación revisar el captchap que se muestra. generar consultas en intervalo de tiempos para no generar algun tipo de laerta, dado que se usan logueos del cliente. Dejar usuarios y contraseñas administrables (POS-PRE). Si la fecha de nacimiento del usuario es mayor a 20000131
+y en la base esta como CC y la respuesta no devuelve nada, se puede consultar como TI o RC
+y en la base esta como TI y la respuesta no devuelve nada, se puede consultar como CC o RC
+y en la base esta como RC y la respuesta no devuelve nada, se puede consultar como CC o TI
+Si la respuesta de la consulta es que si se encuentra en Regimen especial, se debe guardar un pdf con el nombre xxxxxxxx_REG010.pdf donde xxxxxx es el número de identificación y el REG010 la EPS, el cual se toma de una tla según el nombre que entrega la consulta del adres, y guardar en la ruta del servidor
+Se debe crear archivo de 7 columnas, para dejar resgitros de la consulta puntual del régimen especial 7 columnas:, Nombre Vigencia, Contrato, Tipo ID contratante, Número ID contratante, Tipo ID beneficiario, Número ID beneficiario, Código Gestion (44 - Consulta Puntual RES) y que se pueda ejecutar por debajo la función de la opción Acreditación - Gestion - Registrar Gestión Búsqueda Puntual</t>
+  </si>
+  <si>
+    <t>29/09/2025 Jennifer - se contextualiza a Jhon lo que se require
+30/09/2025 Jennifer - Radicación requerimiento en la plataforma</t>
+  </si>
+  <si>
+    <t>OPT_15</t>
+  </si>
+  <si>
+    <t>Acreditación - Usuarios Aliansalud subsidiado</t>
+  </si>
+  <si>
+    <t>Al cargar la respuesta del adres de la consulta, si se recibe un usuario en Aliansalud - sbsidiado, se debe identificar en la tabla de afiliados pos como subsidiado - fecha de última consulta. En el proceso diario y de carga de las consultas se debe ajustar que no se puedan acreditas usuarios de Aliansalud que en la base de afiliados pos tengan la marca de subsidiado</t>
+  </si>
+  <si>
+    <t>30/09/2025 Se inicia con el desarrollo, creando campo nuevo que permite la identificación de si el usuario está en contributivo o subsidiado, según resultado de consulta Adres.</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2302,21 +2331,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="10.67"/>
-    <col customWidth="1" min="3" max="3" width="24.11"/>
-    <col customWidth="1" min="4" max="4" width="40.33"/>
+    <col customWidth="1" min="1" max="1" width="8.11"/>
+    <col customWidth="1" min="2" max="2" width="6.67"/>
+    <col customWidth="1" min="3" max="3" width="20.33"/>
+    <col customWidth="1" min="4" max="4" width="63.56"/>
     <col customWidth="1" hidden="1" min="5" max="5" width="19.56"/>
-    <col customWidth="1" min="6" max="6" width="21.78"/>
+    <col customWidth="1" min="6" max="6" width="13.56"/>
     <col customWidth="1" min="7" max="7" width="6.78"/>
-    <col customWidth="1" min="8" max="8" width="8.22"/>
-    <col customWidth="1" min="9" max="9" width="12.89"/>
-    <col customWidth="1" min="10" max="10" width="12.22"/>
-    <col customWidth="1" min="11" max="11" width="12.0"/>
-    <col customWidth="1" min="12" max="12" width="11.78"/>
-    <col customWidth="1" min="13" max="13" width="8.78"/>
-    <col customWidth="1" min="14" max="14" width="11.0"/>
-    <col customWidth="1" min="15" max="15" width="17.22"/>
+    <col customWidth="1" min="8" max="8" width="5.11"/>
+    <col customWidth="1" min="9" max="12" width="9.22"/>
+    <col customWidth="1" min="13" max="13" width="5.11"/>
+    <col customWidth="1" min="14" max="15" width="9.22"/>
     <col customWidth="1" min="16" max="16" width="33.44"/>
     <col customWidth="1" min="17" max="17" width="8.0"/>
     <col customWidth="1" min="18" max="39" width="10.56"/>
@@ -2794,7 +2819,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32790</v>
+        <v>32792</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2856,7 +2881,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="24">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>32790</v>
+        <v>32792</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -3140,7 +3165,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3418,7 +3443,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32790</v>
+        <v>32792</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3844,7 +3869,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3984,7 +4009,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4092,12 +4117,14 @@
       <c r="AM25" s="42"/>
     </row>
     <row r="26">
-      <c r="A26" s="13"/>
+      <c r="A26" s="13" t="s">
+        <v>107</v>
+      </c>
       <c r="B26" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="17"/>
@@ -4114,7 +4141,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32790</v>
+        <v>32792</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4150,13 +4177,13 @@
         <v>17</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="33" t="s">
@@ -4189,7 +4216,7 @@
         <v>45912.0</v>
       </c>
       <c r="P27" s="40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q27" s="41" t="b">
         <v>1</v>
@@ -4225,10 +4252,10 @@
         <v>315.0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="18" t="s">
@@ -4241,7 +4268,7 @@
         <v>2.0</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J28" s="22">
         <v>45923.0</v>
@@ -4252,12 +4279,12 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
       <c r="P28" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Q28" s="26" t="b">
         <v>1</v>
@@ -4293,10 +4320,10 @@
         <v>314.0</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="33" t="s">
@@ -4309,7 +4336,7 @@
         <v>2.0</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J29" s="37">
         <v>45917.0</v>
@@ -4331,7 +4358,7 @@
         <v>45918.0</v>
       </c>
       <c r="P29" s="40" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q29" s="41" t="b">
         <v>1</v>
@@ -4367,10 +4394,10 @@
         <v>313.0</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="18" t="s">
@@ -4383,7 +4410,7 @@
         <v>3.0</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J30" s="22">
         <v>45912.0</v>
@@ -4405,7 +4432,7 @@
         <v>45916.0</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q30" s="26" t="b">
         <v>1</v>
@@ -4438,13 +4465,13 @@
         <v>36</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="33" t="s">
@@ -4479,7 +4506,7 @@
         <v>45923.0</v>
       </c>
       <c r="P31" s="40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q31" s="41" t="b">
         <v>1</v>
@@ -4512,31 +4539,48 @@
         <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="16"/>
+        <v>129</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="E32" s="17"/>
       <c r="F32" s="18" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="G32" s="19">
-        <v>20.0</v>
-      </c>
-      <c r="H32" s="20"/>
+        <v>100.0</v>
+      </c>
+      <c r="H32" s="20">
+        <v>3.0</v>
+      </c>
       <c r="I32" s="21">
         <v>45923.0</v>
       </c>
-      <c r="J32" s="22"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
+      <c r="J32" s="22">
+        <v>45923.0</v>
+      </c>
+      <c r="K32" s="23">
+        <v>45925.0</v>
+      </c>
+      <c r="L32" s="23">
+        <v>45925.0</v>
+      </c>
+      <c r="M32" s="24">
+        <f>IF(ISBLANK(L32), NETWORKDAYS(J32, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J32, L32, Hoja2!$A$1:$A$18))</f>
+        <v>3</v>
+      </c>
+      <c r="N32" s="23">
+        <v>45925.0</v>
+      </c>
+      <c r="O32" s="23">
+        <v>45926.0</v>
+      </c>
       <c r="P32" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Q32" s="26" t="b">
         <v>1</v>
@@ -4569,13 +4613,13 @@
         <v>17</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="33" t="s">
@@ -4599,8 +4643,9 @@
       <c r="L33" s="37">
         <v>45925.0</v>
       </c>
-      <c r="M33" s="37">
-        <v>45925.0</v>
+      <c r="M33" s="39">
+        <f>IF(ISBLANK(L33), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, L33, Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
       </c>
       <c r="N33" s="37">
         <v>45925.0</v>
@@ -4609,7 +4654,7 @@
         <v>45925.0</v>
       </c>
       <c r="P33" s="40" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="Q33" s="41" t="b">
         <v>1</v>
@@ -4638,32 +4683,47 @@
       <c r="AM33" s="42"/>
     </row>
     <row r="34">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="14">
+        <v>316.0</v>
+      </c>
       <c r="C34" s="15" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+        <v>92</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="H34" s="20">
+        <v>10.0</v>
+      </c>
       <c r="I34" s="21">
         <v>45929.0</v>
       </c>
-      <c r="J34" s="22"/>
+      <c r="J34" s="21">
+        <v>45929.0</v>
+      </c>
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
-      <c r="M34" s="24"/>
+      <c r="M34" s="24">
+        <f>IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
+        <v>3</v>
+      </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
-      <c r="P34" s="25"/>
+      <c r="P34" s="25" t="s">
+        <v>138</v>
+      </c>
       <c r="Q34" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -4689,23 +4749,42 @@
       <c r="AM34" s="27"/>
     </row>
     <row r="35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
+      <c r="A35" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>141</v>
+      </c>
       <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="F35" s="33" t="s">
+        <v>92</v>
+      </c>
       <c r="G35" s="34"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="36"/>
+      <c r="I35" s="36">
+        <v>45925.0</v>
+      </c>
       <c r="J35" s="37"/>
       <c r="K35" s="38"/>
       <c r="L35" s="38"/>
-      <c r="M35" s="39"/>
+      <c r="M35" s="39">
+        <f>IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
+        <v>32792</v>
+      </c>
       <c r="N35" s="38"/>
       <c r="O35" s="38"/>
-      <c r="P35" s="40"/>
-      <c r="Q35" s="41"/>
+      <c r="P35" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q35" s="41" t="b">
+        <v>1</v>
+      </c>
       <c r="R35" s="45"/>
       <c r="S35" s="45"/>
       <c r="T35" s="45"/>
@@ -41835,7 +41914,7 @@
       <c r="AM940" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Q$34"/>
+  <autoFilter ref="$A$1:$Q$35"/>
   <conditionalFormatting sqref="B2:B42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(B$2:B$16,B2)&gt;1</formula>
@@ -41845,7 +41924,7 @@
     <dataValidation type="list" allowBlank="1" sqref="F2:F940">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:O26 I27 I28:L32 N28:O32 I33:O33 I34:L940 N34:O940">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:O26 I27 I28:L940 N28:O940">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -41884,7 +41963,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="85" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>2</v>
@@ -41911,13 +41990,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="88" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="K1" s="85" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="L1" s="89" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="M1" s="90"/>
       <c r="N1" s="90"/>
@@ -41936,14 +42015,14 @@
     </row>
     <row r="2">
       <c r="A2" s="91" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C2" s="93"/>
       <c r="D2" s="94" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E2" s="95">
         <v>45526.0</v>
@@ -41957,7 +42036,7 @@
       <c r="J2" s="93"/>
       <c r="K2" s="93"/>
       <c r="L2" s="93" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="M2" s="96"/>
       <c r="N2" s="96"/>
@@ -41976,13 +42055,13 @@
     </row>
     <row r="3">
       <c r="A3" s="97" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B3" s="98" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C3" s="99" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D3" s="99" t="s">
         <v>20</v>
@@ -42006,7 +42085,7 @@
       </c>
       <c r="K3" s="101"/>
       <c r="L3" s="103" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="M3" s="90"/>
       <c r="N3" s="90"/>
@@ -42025,16 +42104,16 @@
     </row>
     <row r="4">
       <c r="A4" s="104" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C4" s="104" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D4" s="106" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E4" s="107">
         <v>45581.0</v>
@@ -42057,7 +42136,7 @@
       </c>
       <c r="K4" s="107"/>
       <c r="L4" s="104" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="M4" s="110"/>
       <c r="N4" s="110"/>
@@ -42076,16 +42155,16 @@
     </row>
     <row r="5">
       <c r="A5" s="89" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D5" s="111" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E5" s="100">
         <v>45572.0</v>
@@ -42106,7 +42185,7 @@
       </c>
       <c r="K5" s="100"/>
       <c r="L5" s="103" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="M5" s="90"/>
       <c r="N5" s="90"/>
@@ -42125,16 +42204,16 @@
     </row>
     <row r="6">
       <c r="A6" s="112" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B6" s="112" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E6" s="113">
         <v>45602.0</v>
@@ -42155,7 +42234,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="114" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="M6" s="115"/>
       <c r="N6" s="116"/>
@@ -42174,16 +42253,16 @@
     </row>
     <row r="7">
       <c r="A7" s="89" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C7" s="117" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="111" t="s">
         <v>161</v>
-      </c>
-      <c r="D7" s="111" t="s">
-        <v>154</v>
       </c>
       <c r="E7" s="100">
         <v>45589.0</v>
@@ -42204,7 +42283,7 @@
       </c>
       <c r="K7" s="111"/>
       <c r="L7" s="119" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="M7" s="120"/>
       <c r="N7" s="120"/>
@@ -42223,14 +42302,14 @@
     </row>
     <row r="8">
       <c r="A8" s="121" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B8" s="122" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C8" s="123"/>
       <c r="D8" s="123" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E8" s="124">
         <v>45603.0</v>
@@ -42251,7 +42330,7 @@
       </c>
       <c r="K8" s="124"/>
       <c r="L8" s="126" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="M8" s="90"/>
       <c r="N8" s="90"/>
@@ -42270,16 +42349,16 @@
     </row>
     <row r="9">
       <c r="A9" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B9" s="128" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C9" s="129" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E9" s="131">
         <v>45671.0</v>
@@ -42288,7 +42367,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="129" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H9" s="131">
         <v>45680.0</v>
@@ -42302,7 +42381,7 @@
       </c>
       <c r="K9" s="129"/>
       <c r="L9" s="133" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M9" s="134"/>
       <c r="N9" s="134"/>
@@ -42321,14 +42400,14 @@
     </row>
     <row r="10">
       <c r="A10" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B10" s="135"/>
       <c r="C10" s="133" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D10" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E10" s="131">
         <v>45671.0</v>
@@ -42347,7 +42426,7 @@
       <c r="J10" s="129"/>
       <c r="K10" s="129"/>
       <c r="L10" s="133" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M10" s="134"/>
       <c r="N10" s="134"/>
@@ -42366,14 +42445,14 @@
     </row>
     <row r="11">
       <c r="A11" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B11" s="135"/>
       <c r="C11" s="133" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E11" s="131">
         <v>45671.0</v>
@@ -42392,7 +42471,7 @@
       <c r="J11" s="129"/>
       <c r="K11" s="129"/>
       <c r="L11" s="133" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M11" s="134"/>
       <c r="N11" s="134"/>
@@ -42411,14 +42490,14 @@
     </row>
     <row r="12">
       <c r="A12" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B12" s="135"/>
       <c r="C12" s="133" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D12" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E12" s="131">
         <v>45671.0</v>
@@ -42437,7 +42516,7 @@
       <c r="J12" s="129"/>
       <c r="K12" s="129"/>
       <c r="L12" s="133" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M12" s="134"/>
       <c r="N12" s="134"/>
@@ -42456,14 +42535,14 @@
     </row>
     <row r="13">
       <c r="A13" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B13" s="135"/>
       <c r="C13" s="133" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="130" t="s">
         <v>176</v>
-      </c>
-      <c r="D13" s="130" t="s">
-        <v>169</v>
       </c>
       <c r="E13" s="131">
         <v>45671.0</v>
@@ -42482,7 +42561,7 @@
       <c r="J13" s="129"/>
       <c r="K13" s="129"/>
       <c r="L13" s="133" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M13" s="134"/>
       <c r="N13" s="134"/>
@@ -42501,14 +42580,14 @@
     </row>
     <row r="14">
       <c r="A14" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B14" s="135"/>
       <c r="C14" s="133" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D14" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E14" s="131">
         <v>45671.0</v>
@@ -42527,7 +42606,7 @@
       <c r="J14" s="129"/>
       <c r="K14" s="129"/>
       <c r="L14" s="129" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="M14" s="134"/>
       <c r="N14" s="134"/>
@@ -42546,14 +42625,14 @@
     </row>
     <row r="15">
       <c r="A15" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B15" s="135"/>
       <c r="C15" s="133" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D15" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E15" s="131">
         <v>45671.0</v>
@@ -42572,7 +42651,7 @@
       <c r="J15" s="129"/>
       <c r="K15" s="129"/>
       <c r="L15" s="129" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="M15" s="134"/>
       <c r="N15" s="134"/>
@@ -42591,14 +42670,14 @@
     </row>
     <row r="16">
       <c r="A16" s="127" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B16" s="136"/>
       <c r="C16" s="137" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D16" s="130" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E16" s="131">
         <v>45681.0</v>
@@ -42617,7 +42696,7 @@
       <c r="J16" s="129"/>
       <c r="K16" s="129"/>
       <c r="L16" s="133" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="M16" s="134"/>
       <c r="N16" s="134"/>
@@ -49153,7 +49232,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="134" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49161,7 +49240,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49169,7 +49248,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="134" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49177,7 +49256,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="134" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49185,7 +49264,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="134" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49193,7 +49272,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="134" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49201,7 +49280,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="134" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49209,7 +49288,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="134" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49217,7 +49296,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="134" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49225,7 +49304,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="134" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49233,7 +49312,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="134" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49241,7 +49320,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="134" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49249,7 +49328,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="134" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49257,7 +49336,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="134" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49265,7 +49344,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="134" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49273,7 +49352,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="134" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49281,7 +49360,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="134" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49289,7 +49368,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="134" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50305,7 +50384,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="139" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B1" s="134"/>
       <c r="C1" s="134"/>
@@ -50363,7 +50442,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="140" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B3" s="141">
         <v>45596.0</v>
@@ -50656,261 +50735,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="144" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B4" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C4" s="146" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="N4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O4" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P4" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U4" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="V4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE4" s="149" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AF4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL4" s="149" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="AM4" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AN4" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AO4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP4" s="149" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="AQ4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS4" s="149" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="AT4" s="150" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AV4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY4" s="149" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="AZ4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI4" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ4" s="149" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="BK4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BL4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BM4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BN4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BO4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BP4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BQ4" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BL4" s="148" t="s">
+      <c r="BS4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BM4" s="148" t="s">
+      <c r="BT4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BN4" s="148" t="s">
+      <c r="BU4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BO4" s="148" t="s">
+      <c r="BV4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BP4" s="148" t="s">
+      <c r="BW4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BQ4" s="148" t="s">
+      <c r="BX4" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BR4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BS4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BT4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BU4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BV4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BW4" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="BX4" s="147" t="s">
-        <v>202</v>
-      </c>
       <c r="BY4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CD4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG4" s="147"/>
       <c r="CH4" s="147"/>
       <c r="CI4" s="149" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="CJ4" s="147"/>
       <c r="CK4" s="147"/>
@@ -50922,249 +51001,249 @@
       <c r="CQ4" s="147"/>
       <c r="CR4" s="147"/>
       <c r="CS4" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="144" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B5" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L5" s="147" t="s">
+        <v>216</v>
+      </c>
+      <c r="M5" s="147" t="s">
+        <v>216</v>
+      </c>
+      <c r="N5" s="147" t="s">
+        <v>216</v>
+      </c>
+      <c r="O5" s="147" t="s">
+        <v>216</v>
+      </c>
+      <c r="P5" s="148" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q5" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="147" t="s">
+      <c r="R5" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="N5" s="147" t="s">
+      <c r="S5" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="O5" s="147" t="s">
+      <c r="T5" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="P5" s="148" t="s">
+      <c r="U5" s="148" t="s">
         <v>209</v>
       </c>
-      <c r="Q5" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="R5" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="S5" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="T5" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="U5" s="148" t="s">
-        <v>202</v>
-      </c>
       <c r="V5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE5" s="151"/>
       <c r="AF5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL5" s="151"/>
       <c r="AM5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP5" s="151"/>
       <c r="AQ5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AR5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AS5" s="151"/>
       <c r="AT5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AU5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AV5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AW5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AX5" s="147" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AY5" s="151"/>
       <c r="AZ5" s="147" t="s">
+        <v>216</v>
+      </c>
+      <c r="BA5" s="147" t="s">
         <v>209</v>
       </c>
-      <c r="BA5" s="147" t="s">
-        <v>202</v>
-      </c>
       <c r="BB5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI5" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ5" s="151"/>
       <c r="BK5" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL5" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN5" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BP5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CD5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG5" s="147"/>
       <c r="CH5" s="147"/>
@@ -51179,249 +51258,249 @@
       <c r="CQ5" s="147"/>
       <c r="CR5" s="147"/>
       <c r="CS5" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="144" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B6" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K6" s="152" t="s">
+        <v>218</v>
+      </c>
+      <c r="L6" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="M6" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="O6" s="147" t="s">
         <v>211</v>
       </c>
-      <c r="L6" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="M6" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="N6" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="O6" s="147" t="s">
-        <v>204</v>
-      </c>
       <c r="P6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="V6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE6" s="151"/>
       <c r="AF6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL6" s="151"/>
       <c r="AM6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP6" s="151"/>
       <c r="AQ6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS6" s="151"/>
       <c r="AT6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AV6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY6" s="151"/>
       <c r="AZ6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ6" s="151"/>
       <c r="BK6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM6" s="147" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="BN6" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BP6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CD6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG6" s="147"/>
       <c r="CH6" s="147"/>
@@ -51436,198 +51515,198 @@
       <c r="CQ6" s="147"/>
       <c r="CR6" s="147"/>
       <c r="CS6" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="144" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B7" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L7" s="152" t="s">
+        <v>218</v>
+      </c>
+      <c r="M7" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="N7" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="O7" s="147" t="s">
         <v>211</v>
       </c>
-      <c r="M7" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="N7" s="147" t="s">
-        <v>202</v>
-      </c>
-      <c r="O7" s="147" t="s">
-        <v>204</v>
-      </c>
       <c r="P7" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U7" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z7" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AA7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE7" s="151"/>
       <c r="AF7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL7" s="151"/>
       <c r="AM7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP7" s="151"/>
       <c r="AQ7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS7" s="151"/>
       <c r="AT7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU7" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AV7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY7" s="151"/>
       <c r="AZ7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI7" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ7" s="151"/>
       <c r="BK7" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL7" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN7" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO7" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BP7" s="147"/>
       <c r="BQ7" s="147"/>
@@ -51635,16 +51714,16 @@
       <c r="BS7" s="147"/>
       <c r="BT7" s="147"/>
       <c r="BU7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX7" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY7" s="147"/>
       <c r="BZ7" s="147"/>
@@ -51670,220 +51749,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="144" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="B8" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L8" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="M8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="N8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O8" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="V8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W8" s="147" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="X8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB8" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AC8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE8" s="151"/>
       <c r="AF8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL8" s="151"/>
       <c r="AM8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN8" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AO8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP8" s="151"/>
       <c r="AQ8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS8" s="151"/>
       <c r="AT8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AV8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY8" s="151"/>
       <c r="AZ8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG8" s="147" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="BH8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ8" s="151"/>
       <c r="BK8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN8" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BP8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW8" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX8" s="147" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="BY8" s="147"/>
       <c r="BZ8" s="147"/>
@@ -51909,244 +51988,244 @@
     </row>
     <row r="9">
       <c r="A9" s="144" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B9" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="N9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O9" s="152" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="P9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="V9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE9" s="151"/>
       <c r="AF9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL9" s="151"/>
       <c r="AM9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP9" s="151"/>
       <c r="AQ9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS9" s="151"/>
       <c r="AT9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AV9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY9" s="151"/>
       <c r="AZ9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ9" s="151"/>
       <c r="BK9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN9" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BP9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CD9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG9" s="147"/>
       <c r="CH9" s="147"/>
@@ -52161,249 +52240,249 @@
       <c r="CQ9" s="147"/>
       <c r="CR9" s="147"/>
       <c r="CS9" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="144" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B10" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="L10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="N10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="O10" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P10" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Q10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="R10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="T10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="U10" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="V10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AE10" s="151"/>
       <c r="AF10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AL10" s="151"/>
       <c r="AM10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AN10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP10" s="151"/>
       <c r="AQ10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS10" s="151"/>
       <c r="AT10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AV10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY10" s="151"/>
       <c r="AZ10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BA10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BB10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BC10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BD10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BE10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BF10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BG10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BH10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI10" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ10" s="151"/>
       <c r="BK10" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL10" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN10" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BP10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW10" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BX10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CD10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG10" s="147"/>
       <c r="CH10" s="147"/>
@@ -52418,249 +52497,249 @@
       <c r="CQ10" s="147"/>
       <c r="CR10" s="147"/>
       <c r="CS10" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="144" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B11" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="H11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J11" s="147" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="K11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="L11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="N11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O11" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P11" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="R11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="S11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="T11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="U11" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="V11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Y11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Z11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AB11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AC11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AE11" s="151"/>
       <c r="AF11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AG11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AH11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AI11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL11" s="151"/>
       <c r="AM11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AN11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AO11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AP11" s="151"/>
       <c r="AQ11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AR11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AS11" s="151"/>
       <c r="AT11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AU11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AV11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AW11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AY11" s="151"/>
       <c r="AZ11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BA11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BB11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BC11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BE11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BF11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BG11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BH11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI11" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BJ11" s="151"/>
       <c r="BK11" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BL11" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BM11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN11" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BO11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BP11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BQ11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BR11" s="147" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="BS11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BT11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BU11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BX11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BY11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CA11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CB11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CC11" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CD11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG11" s="147"/>
       <c r="CH11" s="147"/>
@@ -52675,249 +52754,249 @@
       <c r="CQ11" s="147"/>
       <c r="CR11" s="147"/>
       <c r="CS11" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="144" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B12" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="G12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="H12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="L12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="N12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="O12" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P12" s="148" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="Q12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="R12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="S12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="T12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="U12" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="V12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="W12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="X12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Y12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Z12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AA12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AB12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AC12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AE12" s="151"/>
       <c r="AF12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AG12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AH12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AI12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AJ12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AK12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AL12" s="151"/>
       <c r="AM12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AN12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AO12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AP12" s="151"/>
       <c r="AQ12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AR12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AS12" s="151"/>
       <c r="AT12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AU12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AV12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AW12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AX12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AY12" s="151"/>
       <c r="AZ12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BA12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BB12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BC12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BD12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BE12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BF12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BG12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BH12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BI12" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BJ12" s="151"/>
       <c r="BK12" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BL12" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BM12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BN12" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BO12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BP12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BQ12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BR12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BS12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BT12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BU12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BV12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BW12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BX12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BY12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="BZ12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CA12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CB12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CC12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CD12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CE12" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CG12" s="147"/>
       <c r="CH12" s="147"/>
@@ -52932,249 +53011,249 @@
       <c r="CQ12" s="147"/>
       <c r="CR12" s="147"/>
       <c r="CS12" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="144" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B13" s="145" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="F13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="G13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="H13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="I13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="K13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="L13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="M13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="N13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="O13" s="147" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="P13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Q13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="R13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="S13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="T13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="U13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="V13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="W13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="X13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Y13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="Z13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AA13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AB13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AC13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AD13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AE13" s="153"/>
       <c r="AF13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AG13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AH13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AI13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="AJ13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AK13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AL13" s="153"/>
       <c r="AM13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AN13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AO13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AP13" s="153"/>
       <c r="AQ13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AR13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AS13" s="153"/>
       <c r="AT13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AU13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AV13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AW13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AX13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AY13" s="153"/>
       <c r="AZ13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BA13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BB13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BC13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BD13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BE13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BF13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BG13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BH13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BI13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BJ13" s="153"/>
       <c r="BK13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BL13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BM13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BN13" s="148" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BO13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BP13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BQ13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BR13" s="147" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="BS13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BT13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BU13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BV13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BW13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BX13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BY13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="BZ13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CA13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CB13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CC13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="CD13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CE13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CF13" s="147" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="CG13" s="147"/>
       <c r="CH13" s="147"/>
@@ -53189,7 +53268,7 @@
       <c r="CQ13" s="147"/>
       <c r="CR13" s="147"/>
       <c r="CS13" s="147" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54215,7 +54294,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="154" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B1" s="154" t="s">
         <v>2</v>
@@ -54242,13 +54321,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="158" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="K1" s="159" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="L1" s="157" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="M1" s="160"/>
       <c r="N1" s="160"/>
@@ -54267,10 +54346,10 @@
     </row>
     <row r="2">
       <c r="A2" s="161" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B2" s="162" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C2" s="163"/>
       <c r="D2" s="163" t="s">
@@ -54297,7 +54376,7 @@
       </c>
       <c r="K2" s="166"/>
       <c r="L2" s="167" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="M2" s="160"/>
       <c r="N2" s="160"/>
@@ -54316,13 +54395,13 @@
     </row>
     <row r="3">
       <c r="A3" s="161" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C3" s="169" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D3" s="163" t="s">
         <v>39</v>
@@ -54344,7 +54423,7 @@
       </c>
       <c r="K3" s="164"/>
       <c r="L3" s="167" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="M3" s="170"/>
       <c r="N3" s="160"/>
@@ -54363,11 +54442,11 @@
     </row>
     <row r="4">
       <c r="A4" s="161" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B4" s="151"/>
       <c r="C4" s="171" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D4" s="163" t="s">
         <v>39</v>
@@ -54389,7 +54468,7 @@
       </c>
       <c r="K4" s="172"/>
       <c r="L4" s="175" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="M4" s="170"/>
       <c r="N4" s="160"/>
@@ -54408,13 +54487,13 @@
     </row>
     <row r="5">
       <c r="A5" s="161" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B5" s="157" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C5" s="163" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D5" s="163" t="s">
         <v>39</v>
@@ -54436,7 +54515,7 @@
       </c>
       <c r="K5" s="164"/>
       <c r="L5" s="167" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="M5" s="170"/>
       <c r="N5" s="160"/>

</xml_diff>